<commit_message>
Updating chart till Presentation date
</commit_message>
<xml_diff>
--- a/documentation/Charts/Charts-WIP.xlsx
+++ b/documentation/Charts/Charts-WIP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rex\Desktop\Project template code\Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C305F1-9953-40E0-A6BD-2DDCE96FD6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F88D29-40FC-4D35-8A0D-98720055CBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{5FED8FEB-A2F0-45E6-B7D6-62982F9FC7E5}"/>
   </bookViews>
@@ -1313,21 +1313,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1400,9 +1385,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1415,17 +1397,11 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1441,6 +1417,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4414,8 +4414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3693011-238F-42BC-B2CC-2AF5AE5811AA}">
   <dimension ref="B4:M87"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U39" sqref="U39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4425,56 +4425,56 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="73" t="s">
+      <c r="D5" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="73" t="s">
+      <c r="G5" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="73" t="s">
+      <c r="I5" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="73" t="s">
+      <c r="J5" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="73" t="s">
+      <c r="K5" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L5" s="73" t="s">
+      <c r="L5" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M5" s="73" t="s">
+      <c r="M5" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -4631,113 +4631,113 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="70">
         <f>SUM(M6:M9)</f>
         <v>40</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="78"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="72"/>
+      <c r="I10" s="72"/>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="73"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="75">
+      <c r="C11" s="70">
         <f>SUM(C6:L9)</f>
         <v>56</v>
       </c>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="80"/>
+      <c r="D11" s="74"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="75"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="74" t="s">
+      <c r="B12" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="75">
+      <c r="C12" s="70">
         <f>SUM(C10,-(C11))</f>
         <v>-16</v>
       </c>
-      <c r="D12" s="81"/>
-      <c r="E12" s="82"/>
-      <c r="F12" s="82"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="82"/>
-      <c r="J12" s="82"/>
-      <c r="K12" s="82"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="83"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="78"/>
     </row>
     <row r="14" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="67"/>
-      <c r="I14" s="67"/>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="73" t="s">
+      <c r="C15" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G15" s="73" t="s">
+      <c r="G15" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="73" t="s">
+      <c r="H15" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I15" s="73" t="s">
+      <c r="I15" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="73" t="s">
+      <c r="J15" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="73" t="s">
+      <c r="K15" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L15" s="73" t="s">
+      <c r="L15" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M15" s="73" t="s">
+      <c r="M15" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5008,113 +5008,113 @@
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="75">
+      <c r="C23" s="70">
         <f>SUM(M16:M22)</f>
         <v>52</v>
       </c>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="78"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="72"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="72"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="73"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="74" t="s">
+      <c r="B24" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="75">
+      <c r="C24" s="70">
         <f>SUM(C16:L22)</f>
         <v>71</v>
       </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
-      <c r="I24" s="79"/>
-      <c r="J24" s="79"/>
-      <c r="K24" s="79"/>
-      <c r="L24" s="79"/>
-      <c r="M24" s="80"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="74"/>
+      <c r="L24" s="74"/>
+      <c r="M24" s="75"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="75">
+      <c r="C25" s="70">
         <f>SUM(C23,-(C24))</f>
         <v>-19</v>
       </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="83"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="77"/>
+      <c r="I25" s="77"/>
+      <c r="J25" s="77"/>
+      <c r="K25" s="77"/>
+      <c r="L25" s="77"/>
+      <c r="M25" s="78"/>
     </row>
     <row r="27" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B27" s="67" t="s">
+      <c r="B27" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
-      <c r="M27" s="67"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="102"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="72" t="s">
+      <c r="B28" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="73" t="s">
+      <c r="C28" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="73" t="s">
+      <c r="D28" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F28" s="73" t="s">
+      <c r="F28" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G28" s="73" t="s">
+      <c r="G28" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H28" s="73" t="s">
+      <c r="H28" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I28" s="73" t="s">
+      <c r="I28" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J28" s="73" t="s">
+      <c r="J28" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K28" s="73" t="s">
+      <c r="K28" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L28" s="73" t="s">
+      <c r="L28" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M28" s="73" t="s">
+      <c r="M28" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5128,7 +5128,9 @@
       <c r="D29" s="12">
         <v>2</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="12">
+        <v>1</v>
+      </c>
       <c r="F29" s="12"/>
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
@@ -5405,117 +5407,117 @@
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="74" t="s">
+      <c r="B42" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="75">
+      <c r="C42" s="70">
         <f>SUM(M29:M41)</f>
         <v>73</v>
       </c>
-      <c r="D42" s="76"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
-      <c r="I42" s="77"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="77"/>
-      <c r="L42" s="77"/>
-      <c r="M42" s="78"/>
+      <c r="D42" s="71"/>
+      <c r="E42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="73"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="75">
+      <c r="C43" s="70">
         <f>SUM(C29:L41)</f>
-        <v>4</v>
-      </c>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="80"/>
+        <v>5</v>
+      </c>
+      <c r="D43" s="74"/>
+      <c r="E43" s="74"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="74"/>
+      <c r="M43" s="75"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B44" s="74" t="s">
+      <c r="B44" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="75">
+      <c r="C44" s="70">
         <f>SUM(C42,-(C43))</f>
-        <v>69</v>
-      </c>
-      <c r="D44" s="81"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="82"/>
-      <c r="K44" s="82"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="83"/>
+        <v>68</v>
+      </c>
+      <c r="D44" s="76"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="77"/>
+      <c r="G44" s="77"/>
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="77"/>
+      <c r="K44" s="77"/>
+      <c r="L44" s="77"/>
+      <c r="M44" s="78"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B46" s="67" t="s">
+      <c r="B46" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="67"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
-      <c r="K46" s="67"/>
-      <c r="L46" s="67"/>
-      <c r="M46" s="67"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="102"/>
+      <c r="E46" s="102"/>
+      <c r="F46" s="102"/>
+      <c r="G46" s="102"/>
+      <c r="H46" s="102"/>
+      <c r="I46" s="102"/>
+      <c r="J46" s="102"/>
+      <c r="K46" s="102"/>
+      <c r="L46" s="102"/>
+      <c r="M46" s="102"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B47" s="72" t="s">
+      <c r="B47" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C47" s="73" t="s">
+      <c r="C47" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="73" t="s">
+      <c r="D47" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="73" t="s">
+      <c r="E47" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F47" s="73" t="s">
+      <c r="F47" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G47" s="73" t="s">
+      <c r="G47" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H47" s="73" t="s">
+      <c r="H47" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="73" t="s">
+      <c r="I47" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J47" s="73" t="s">
+      <c r="J47" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K47" s="73" t="s">
+      <c r="K47" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L47" s="73" t="s">
+      <c r="L47" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M47" s="73" t="s">
+      <c r="M47" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5682,113 +5684,113 @@
       </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="74" t="s">
+      <c r="B57" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="75">
+      <c r="C57" s="70">
         <f>SUM(M48:M55)</f>
         <v>60</v>
       </c>
-      <c r="D57" s="76"/>
-      <c r="E57" s="77"/>
-      <c r="F57" s="77"/>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="78"/>
+      <c r="D57" s="71"/>
+      <c r="E57" s="72"/>
+      <c r="F57" s="72"/>
+      <c r="G57" s="72"/>
+      <c r="H57" s="72"/>
+      <c r="I57" s="72"/>
+      <c r="J57" s="72"/>
+      <c r="K57" s="72"/>
+      <c r="L57" s="72"/>
+      <c r="M57" s="73"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C58" s="75">
+      <c r="C58" s="70">
         <f>SUM(C48:L55)</f>
         <v>0</v>
       </c>
-      <c r="D58" s="79"/>
-      <c r="E58" s="79"/>
-      <c r="F58" s="79"/>
-      <c r="G58" s="79"/>
-      <c r="H58" s="79"/>
-      <c r="I58" s="79"/>
-      <c r="J58" s="79"/>
-      <c r="K58" s="79"/>
-      <c r="L58" s="79"/>
-      <c r="M58" s="80"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="74"/>
+      <c r="K58" s="74"/>
+      <c r="L58" s="74"/>
+      <c r="M58" s="75"/>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="74" t="s">
+      <c r="B59" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C59" s="75">
+      <c r="C59" s="70">
         <f>SUM(C57,-(C58))</f>
         <v>60</v>
       </c>
-      <c r="D59" s="81"/>
-      <c r="E59" s="82"/>
-      <c r="F59" s="82"/>
-      <c r="G59" s="82"/>
-      <c r="H59" s="82"/>
-      <c r="I59" s="82"/>
-      <c r="J59" s="82"/>
-      <c r="K59" s="82"/>
-      <c r="L59" s="82"/>
-      <c r="M59" s="83"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="77"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="77"/>
+      <c r="I59" s="77"/>
+      <c r="J59" s="77"/>
+      <c r="K59" s="77"/>
+      <c r="L59" s="77"/>
+      <c r="M59" s="78"/>
     </row>
     <row r="61" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B61" s="68" t="s">
+      <c r="B61" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="69"/>
-      <c r="D61" s="69"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="69"/>
-      <c r="H61" s="69"/>
-      <c r="I61" s="69"/>
-      <c r="J61" s="69"/>
-      <c r="K61" s="69"/>
-      <c r="L61" s="69"/>
-      <c r="M61" s="70"/>
+      <c r="C61" s="104"/>
+      <c r="D61" s="104"/>
+      <c r="E61" s="104"/>
+      <c r="F61" s="104"/>
+      <c r="G61" s="104"/>
+      <c r="H61" s="104"/>
+      <c r="I61" s="104"/>
+      <c r="J61" s="104"/>
+      <c r="K61" s="104"/>
+      <c r="L61" s="104"/>
+      <c r="M61" s="105"/>
     </row>
     <row r="62" spans="2:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="73" t="s">
+      <c r="C62" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D62" s="73" t="s">
+      <c r="D62" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E62" s="73" t="s">
+      <c r="E62" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F62" s="73" t="s">
+      <c r="F62" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G62" s="73" t="s">
+      <c r="G62" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H62" s="73" t="s">
+      <c r="H62" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I62" s="73" t="s">
+      <c r="I62" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J62" s="73" t="s">
+      <c r="J62" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K62" s="73" t="s">
+      <c r="K62" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L62" s="73" t="s">
+      <c r="L62" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M62" s="73" t="s">
+      <c r="M62" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5937,113 +5939,113 @@
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="74" t="s">
+      <c r="B71" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C71" s="75">
+      <c r="C71" s="70">
         <f>SUM(M63:M70)</f>
         <v>65</v>
       </c>
-      <c r="D71" s="76"/>
-      <c r="E71" s="77"/>
-      <c r="F71" s="77"/>
-      <c r="G71" s="77"/>
-      <c r="H71" s="77"/>
-      <c r="I71" s="77"/>
-      <c r="J71" s="77"/>
-      <c r="K71" s="77"/>
-      <c r="L71" s="77"/>
-      <c r="M71" s="78"/>
+      <c r="D71" s="71"/>
+      <c r="E71" s="72"/>
+      <c r="F71" s="72"/>
+      <c r="G71" s="72"/>
+      <c r="H71" s="72"/>
+      <c r="I71" s="72"/>
+      <c r="J71" s="72"/>
+      <c r="K71" s="72"/>
+      <c r="L71" s="72"/>
+      <c r="M71" s="73"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="74" t="s">
+      <c r="B72" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="75">
+      <c r="C72" s="70">
         <f>SUM(C63:L70)</f>
         <v>0</v>
       </c>
-      <c r="D72" s="79"/>
-      <c r="E72" s="79"/>
-      <c r="F72" s="79"/>
-      <c r="G72" s="79"/>
-      <c r="H72" s="79"/>
-      <c r="I72" s="79"/>
-      <c r="J72" s="79"/>
-      <c r="K72" s="79"/>
-      <c r="L72" s="79"/>
-      <c r="M72" s="80"/>
+      <c r="D72" s="74"/>
+      <c r="E72" s="74"/>
+      <c r="F72" s="74"/>
+      <c r="G72" s="74"/>
+      <c r="H72" s="74"/>
+      <c r="I72" s="74"/>
+      <c r="J72" s="74"/>
+      <c r="K72" s="74"/>
+      <c r="L72" s="74"/>
+      <c r="M72" s="75"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="74" t="s">
+      <c r="B73" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C73" s="75">
+      <c r="C73" s="70">
         <f>SUM(C71,-(C72))</f>
         <v>65</v>
       </c>
-      <c r="D73" s="81"/>
-      <c r="E73" s="82"/>
-      <c r="F73" s="82"/>
-      <c r="G73" s="82"/>
-      <c r="H73" s="82"/>
-      <c r="I73" s="82"/>
-      <c r="J73" s="82"/>
-      <c r="K73" s="82"/>
-      <c r="L73" s="82"/>
-      <c r="M73" s="83"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="77"/>
+      <c r="F73" s="77"/>
+      <c r="G73" s="77"/>
+      <c r="H73" s="77"/>
+      <c r="I73" s="77"/>
+      <c r="J73" s="77"/>
+      <c r="K73" s="77"/>
+      <c r="L73" s="77"/>
+      <c r="M73" s="78"/>
     </row>
     <row r="75" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B75" s="68" t="s">
+      <c r="B75" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="69"/>
-      <c r="D75" s="69"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="69"/>
-      <c r="I75" s="69"/>
-      <c r="J75" s="69"/>
-      <c r="K75" s="69"/>
-      <c r="L75" s="69"/>
-      <c r="M75" s="70"/>
+      <c r="C75" s="104"/>
+      <c r="D75" s="104"/>
+      <c r="E75" s="104"/>
+      <c r="F75" s="104"/>
+      <c r="G75" s="104"/>
+      <c r="H75" s="104"/>
+      <c r="I75" s="104"/>
+      <c r="J75" s="104"/>
+      <c r="K75" s="104"/>
+      <c r="L75" s="104"/>
+      <c r="M75" s="105"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="72" t="s">
+      <c r="B76" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="73" t="s">
+      <c r="C76" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D76" s="73" t="s">
+      <c r="D76" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="E76" s="73" t="s">
+      <c r="E76" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="F76" s="73" t="s">
+      <c r="F76" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="G76" s="73" t="s">
+      <c r="G76" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H76" s="73" t="s">
+      <c r="H76" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="I76" s="73" t="s">
+      <c r="I76" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="J76" s="73" t="s">
+      <c r="J76" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="K76" s="73" t="s">
+      <c r="K76" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="L76" s="73" t="s">
+      <c r="L76" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="M76" s="73" t="s">
+      <c r="M76" s="68" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6192,61 +6194,61 @@
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B85" s="74" t="s">
+      <c r="B85" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="C85" s="75">
+      <c r="C85" s="70">
         <f>SUM(M77:M84)</f>
         <v>60</v>
       </c>
-      <c r="D85" s="76"/>
-      <c r="E85" s="77"/>
-      <c r="F85" s="77"/>
-      <c r="G85" s="77"/>
-      <c r="H85" s="77"/>
-      <c r="I85" s="77"/>
-      <c r="J85" s="77"/>
-      <c r="K85" s="77"/>
-      <c r="L85" s="77"/>
-      <c r="M85" s="78"/>
+      <c r="D85" s="71"/>
+      <c r="E85" s="72"/>
+      <c r="F85" s="72"/>
+      <c r="G85" s="72"/>
+      <c r="H85" s="72"/>
+      <c r="I85" s="72"/>
+      <c r="J85" s="72"/>
+      <c r="K85" s="72"/>
+      <c r="L85" s="72"/>
+      <c r="M85" s="73"/>
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="74" t="s">
+      <c r="B86" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="C86" s="75">
+      <c r="C86" s="70">
         <f>SUM(C77:L84)</f>
         <v>0</v>
       </c>
-      <c r="D86" s="79"/>
-      <c r="E86" s="79"/>
-      <c r="F86" s="79"/>
-      <c r="G86" s="79"/>
-      <c r="H86" s="79"/>
-      <c r="I86" s="79"/>
-      <c r="J86" s="79"/>
-      <c r="K86" s="79"/>
-      <c r="L86" s="79"/>
-      <c r="M86" s="80"/>
+      <c r="D86" s="74"/>
+      <c r="E86" s="74"/>
+      <c r="F86" s="74"/>
+      <c r="G86" s="74"/>
+      <c r="H86" s="74"/>
+      <c r="I86" s="74"/>
+      <c r="J86" s="74"/>
+      <c r="K86" s="74"/>
+      <c r="L86" s="74"/>
+      <c r="M86" s="75"/>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B87" s="74" t="s">
+      <c r="B87" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C87" s="75">
+      <c r="C87" s="70">
         <f>SUM(C85,-(C86))</f>
         <v>60</v>
       </c>
-      <c r="D87" s="81"/>
-      <c r="E87" s="82"/>
-      <c r="F87" s="82"/>
-      <c r="G87" s="82"/>
-      <c r="H87" s="82"/>
-      <c r="I87" s="82"/>
-      <c r="J87" s="82"/>
-      <c r="K87" s="82"/>
-      <c r="L87" s="82"/>
-      <c r="M87" s="83"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="77"/>
+      <c r="F87" s="77"/>
+      <c r="G87" s="77"/>
+      <c r="H87" s="77"/>
+      <c r="I87" s="77"/>
+      <c r="J87" s="77"/>
+      <c r="K87" s="77"/>
+      <c r="L87" s="77"/>
+      <c r="M87" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -6271,7 +6273,7 @@
   <dimension ref="A1:CN92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6345,114 +6347,114 @@
       <c r="F2" s="63"/>
       <c r="G2" s="63"/>
       <c r="H2" s="22"/>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71" t="s">
+      <c r="J2" s="106"/>
+      <c r="K2" s="106"/>
+      <c r="L2" s="106"/>
+      <c r="M2" s="106"/>
+      <c r="N2" s="106"/>
+      <c r="O2" s="106"/>
+      <c r="P2" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71"/>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71" t="s">
+      <c r="Q2" s="106"/>
+      <c r="R2" s="106"/>
+      <c r="S2" s="106"/>
+      <c r="T2" s="106"/>
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="71"/>
-      <c r="AC2" s="71"/>
-      <c r="AD2" s="71" t="s">
+      <c r="X2" s="106"/>
+      <c r="Y2" s="106"/>
+      <c r="Z2" s="106"/>
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="AE2" s="71"/>
-      <c r="AF2" s="71"/>
-      <c r="AG2" s="71"/>
-      <c r="AH2" s="71"/>
-      <c r="AI2" s="71"/>
-      <c r="AJ2" s="71"/>
-      <c r="AK2" s="71" t="s">
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="106"/>
+      <c r="AG2" s="106"/>
+      <c r="AH2" s="106"/>
+      <c r="AI2" s="106"/>
+      <c r="AJ2" s="106"/>
+      <c r="AK2" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="AL2" s="71"/>
-      <c r="AM2" s="71"/>
-      <c r="AN2" s="71"/>
-      <c r="AO2" s="71"/>
-      <c r="AP2" s="71"/>
-      <c r="AQ2" s="71"/>
-      <c r="AR2" s="71" t="s">
+      <c r="AL2" s="106"/>
+      <c r="AM2" s="106"/>
+      <c r="AN2" s="106"/>
+      <c r="AO2" s="106"/>
+      <c r="AP2" s="106"/>
+      <c r="AQ2" s="106"/>
+      <c r="AR2" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="AS2" s="71"/>
-      <c r="AT2" s="71"/>
-      <c r="AU2" s="71"/>
-      <c r="AV2" s="71"/>
-      <c r="AW2" s="71"/>
-      <c r="AX2" s="71"/>
-      <c r="AY2" s="71" t="s">
+      <c r="AS2" s="106"/>
+      <c r="AT2" s="106"/>
+      <c r="AU2" s="106"/>
+      <c r="AV2" s="106"/>
+      <c r="AW2" s="106"/>
+      <c r="AX2" s="106"/>
+      <c r="AY2" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="AZ2" s="71"/>
-      <c r="BA2" s="71"/>
-      <c r="BB2" s="71"/>
-      <c r="BC2" s="71"/>
-      <c r="BD2" s="71"/>
-      <c r="BE2" s="71"/>
-      <c r="BF2" s="71" t="s">
+      <c r="AZ2" s="106"/>
+      <c r="BA2" s="106"/>
+      <c r="BB2" s="106"/>
+      <c r="BC2" s="106"/>
+      <c r="BD2" s="106"/>
+      <c r="BE2" s="106"/>
+      <c r="BF2" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="BG2" s="71"/>
-      <c r="BH2" s="71"/>
-      <c r="BI2" s="71"/>
-      <c r="BJ2" s="71"/>
-      <c r="BK2" s="71"/>
-      <c r="BL2" s="71"/>
-      <c r="BM2" s="71" t="s">
+      <c r="BG2" s="106"/>
+      <c r="BH2" s="106"/>
+      <c r="BI2" s="106"/>
+      <c r="BJ2" s="106"/>
+      <c r="BK2" s="106"/>
+      <c r="BL2" s="106"/>
+      <c r="BM2" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="BN2" s="71"/>
-      <c r="BO2" s="71"/>
-      <c r="BP2" s="71"/>
-      <c r="BQ2" s="71"/>
-      <c r="BR2" s="71"/>
-      <c r="BS2" s="71"/>
-      <c r="BT2" s="71" t="s">
+      <c r="BN2" s="106"/>
+      <c r="BO2" s="106"/>
+      <c r="BP2" s="106"/>
+      <c r="BQ2" s="106"/>
+      <c r="BR2" s="106"/>
+      <c r="BS2" s="106"/>
+      <c r="BT2" s="106" t="s">
         <v>87</v>
       </c>
-      <c r="BU2" s="71"/>
-      <c r="BV2" s="71"/>
-      <c r="BW2" s="71"/>
-      <c r="BX2" s="71"/>
-      <c r="BY2" s="71"/>
-      <c r="BZ2" s="71"/>
-      <c r="CA2" s="71" t="s">
+      <c r="BU2" s="106"/>
+      <c r="BV2" s="106"/>
+      <c r="BW2" s="106"/>
+      <c r="BX2" s="106"/>
+      <c r="BY2" s="106"/>
+      <c r="BZ2" s="106"/>
+      <c r="CA2" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="CB2" s="71"/>
-      <c r="CC2" s="71"/>
-      <c r="CD2" s="71"/>
-      <c r="CE2" s="71"/>
-      <c r="CF2" s="71"/>
-      <c r="CG2" s="71"/>
-      <c r="CH2" s="71" t="s">
+      <c r="CB2" s="106"/>
+      <c r="CC2" s="106"/>
+      <c r="CD2" s="106"/>
+      <c r="CE2" s="106"/>
+      <c r="CF2" s="106"/>
+      <c r="CG2" s="106"/>
+      <c r="CH2" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="CI2" s="71"/>
-      <c r="CJ2" s="71"/>
-      <c r="CK2" s="71"/>
-      <c r="CL2" s="71"/>
-      <c r="CM2" s="71"/>
-      <c r="CN2" s="71"/>
+      <c r="CI2" s="106"/>
+      <c r="CJ2" s="106"/>
+      <c r="CK2" s="106"/>
+      <c r="CL2" s="106"/>
+      <c r="CM2" s="106"/>
+      <c r="CN2" s="106"/>
     </row>
     <row r="3" spans="1:92" s="2" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="64"/>
@@ -6989,13 +6991,13 @@
     </row>
     <row r="5" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="96" t="s">
+      <c r="C5" s="94"/>
+      <c r="D5" s="107" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
+      <c r="E5" s="107"/>
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
       <c r="H5" s="28"/>
       <c r="I5" s="29"/>
       <c r="J5" s="29"/>
@@ -7084,13 +7086,13 @@
     </row>
     <row r="6" spans="1:92" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="98" t="s">
+      <c r="C6" s="91"/>
+      <c r="D6" s="92" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="99"/>
-      <c r="G6" s="99"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
       <c r="H6" s="30"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -7178,24 +7180,24 @@
       <c r="CN6" s="46"/>
     </row>
     <row r="7" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C7" s="84">
+      <c r="C7" s="79">
         <v>1</v>
       </c>
-      <c r="D7" s="85" t="s">
+      <c r="D7" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="81">
         <v>1</v>
       </c>
-      <c r="F7" s="87">
+      <c r="F7" s="82">
         <v>44410</v>
       </c>
-      <c r="G7" s="87">
+      <c r="G7" s="82">
         <v>44411</v>
       </c>
       <c r="H7" s="31"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="105"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
       <c r="K7" s="37"/>
       <c r="L7" s="37"/>
       <c r="M7" s="37"/>
@@ -7280,31 +7282,31 @@
       <c r="CN7" s="46"/>
     </row>
     <row r="8" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C8" s="84">
+      <c r="C8" s="79">
         <v>2</v>
       </c>
-      <c r="D8" s="88" t="s">
+      <c r="D8" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="86">
+      <c r="E8" s="81">
         <v>1</v>
       </c>
-      <c r="F8" s="87">
+      <c r="F8" s="82">
         <v>44410</v>
       </c>
-      <c r="G8" s="87">
+      <c r="G8" s="82">
         <v>44418</v>
       </c>
       <c r="H8" s="32"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="105"/>
+      <c r="I8" s="97"/>
+      <c r="J8" s="97"/>
+      <c r="K8" s="97"/>
+      <c r="L8" s="97"/>
+      <c r="M8" s="97"/>
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
-      <c r="P8" s="105"/>
-      <c r="Q8" s="105"/>
+      <c r="P8" s="97"/>
+      <c r="Q8" s="97"/>
       <c r="R8" s="26"/>
       <c r="S8" s="26"/>
       <c r="T8" s="26"/>
@@ -7382,33 +7384,33 @@
       <c r="CN8" s="46"/>
     </row>
     <row r="9" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C9" s="84">
+      <c r="C9" s="79">
         <v>3</v>
       </c>
-      <c r="D9" s="88" t="s">
+      <c r="D9" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="86">
+      <c r="E9" s="81">
         <v>1</v>
       </c>
-      <c r="F9" s="87">
+      <c r="F9" s="82">
         <v>44413</v>
       </c>
-      <c r="G9" s="87">
+      <c r="G9" s="82">
         <v>44420</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="26"/>
       <c r="J9" s="26"/>
       <c r="K9" s="26"/>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
       <c r="N9" s="26"/>
       <c r="O9" s="26"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
+      <c r="P9" s="97"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="97"/>
+      <c r="S9" s="97"/>
       <c r="T9" s="26"/>
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
@@ -7485,19 +7487,19 @@
     </row>
     <row r="10" spans="1:92" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
-      <c r="C10" s="84">
+      <c r="C10" s="79">
         <v>4</v>
       </c>
-      <c r="D10" s="88" t="s">
+      <c r="D10" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="86">
+      <c r="E10" s="81">
         <v>1</v>
       </c>
-      <c r="F10" s="87">
+      <c r="F10" s="82">
         <v>44419</v>
       </c>
-      <c r="G10" s="87">
+      <c r="G10" s="82">
         <v>44423</v>
       </c>
       <c r="H10" s="32"/>
@@ -7509,10 +7511,10 @@
       <c r="N10" s="26"/>
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="105"/>
-      <c r="S10" s="105"/>
-      <c r="T10" s="105"/>
+      <c r="Q10" s="98"/>
+      <c r="R10" s="97"/>
+      <c r="S10" s="97"/>
+      <c r="T10" s="97"/>
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
       <c r="W10" s="8"/>
@@ -7588,13 +7590,13 @@
     </row>
     <row r="11" spans="1:92" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="96" t="s">
+      <c r="C11" s="91"/>
+      <c r="D11" s="107" t="s">
         <v>90</v>
       </c>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
       <c r="H11" s="30"/>
       <c r="I11" s="26"/>
       <c r="J11" s="26"/>
@@ -7683,15 +7685,15 @@
     </row>
     <row r="12" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="97">
+      <c r="C12" s="91">
         <v>1</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="98"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
       <c r="H12" s="30"/>
       <c r="I12" s="26"/>
       <c r="J12" s="26"/>
@@ -7779,19 +7781,19 @@
       <c r="CN12" s="46"/>
     </row>
     <row r="13" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C13" s="84">
+      <c r="C13" s="79">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="86">
+      <c r="E13" s="81">
         <v>1</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="82">
         <v>44424</v>
       </c>
-      <c r="G13" s="87">
+      <c r="G13" s="82">
         <v>44427</v>
       </c>
       <c r="H13" s="33"/>
@@ -7809,10 +7811,10 @@
       <c r="T13" s="8"/>
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
-      <c r="W13" s="105"/>
-      <c r="X13" s="105"/>
-      <c r="Y13" s="107"/>
-      <c r="Z13" s="107"/>
+      <c r="W13" s="97"/>
+      <c r="X13" s="97"/>
+      <c r="Y13" s="99"/>
+      <c r="Z13" s="99"/>
       <c r="AA13" s="47"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
@@ -7881,19 +7883,19 @@
       <c r="CN13" s="46"/>
     </row>
     <row r="14" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C14" s="84">
+      <c r="C14" s="79">
         <v>1.2</v>
       </c>
-      <c r="D14" s="89" t="s">
+      <c r="D14" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="86">
+      <c r="E14" s="81">
         <v>1</v>
       </c>
-      <c r="F14" s="87">
+      <c r="F14" s="82">
         <v>44424</v>
       </c>
-      <c r="G14" s="87">
+      <c r="G14" s="82">
         <v>44427</v>
       </c>
       <c r="H14" s="33"/>
@@ -7911,10 +7913,10 @@
       <c r="T14" s="8"/>
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
-      <c r="W14" s="107"/>
-      <c r="X14" s="107"/>
-      <c r="Y14" s="107"/>
-      <c r="Z14" s="107"/>
+      <c r="W14" s="99"/>
+      <c r="X14" s="99"/>
+      <c r="Y14" s="99"/>
+      <c r="Z14" s="99"/>
       <c r="AA14" s="47"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
@@ -7983,19 +7985,19 @@
       <c r="CN14" s="46"/>
     </row>
     <row r="15" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C15" s="84">
+      <c r="C15" s="79">
         <v>1.3</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="81">
         <v>1</v>
       </c>
-      <c r="F15" s="87">
+      <c r="F15" s="82">
         <v>44424</v>
       </c>
-      <c r="G15" s="87">
+      <c r="G15" s="82">
         <v>44427</v>
       </c>
       <c r="H15" s="33"/>
@@ -8013,10 +8015,10 @@
       <c r="T15" s="8"/>
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
-      <c r="W15" s="107"/>
-      <c r="X15" s="107"/>
-      <c r="Y15" s="107"/>
-      <c r="Z15" s="107"/>
+      <c r="W15" s="99"/>
+      <c r="X15" s="99"/>
+      <c r="Y15" s="99"/>
+      <c r="Z15" s="99"/>
       <c r="AA15" s="47"/>
       <c r="AB15" s="8"/>
       <c r="AC15" s="8"/>
@@ -8085,19 +8087,19 @@
       <c r="CN15" s="46"/>
     </row>
     <row r="16" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="C16" s="84">
+      <c r="C16" s="79">
         <v>1.4</v>
       </c>
-      <c r="D16" s="89" t="s">
+      <c r="D16" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="86">
+      <c r="E16" s="81">
         <v>1</v>
       </c>
-      <c r="F16" s="87">
+      <c r="F16" s="82">
         <v>44426</v>
       </c>
-      <c r="G16" s="87">
+      <c r="G16" s="82">
         <v>44432</v>
       </c>
       <c r="H16" s="33"/>
@@ -8117,13 +8119,13 @@
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8"/>
-      <c r="Y16" s="107"/>
-      <c r="Z16" s="107"/>
-      <c r="AA16" s="107"/>
+      <c r="Y16" s="99"/>
+      <c r="Z16" s="99"/>
+      <c r="AA16" s="99"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="8"/>
-      <c r="AD16" s="107"/>
-      <c r="AE16" s="107"/>
+      <c r="AD16" s="99"/>
+      <c r="AE16" s="99"/>
       <c r="AF16" s="47"/>
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
@@ -8187,15 +8189,15 @@
       <c r="CN16" s="46"/>
     </row>
     <row r="17" spans="2:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C17" s="97">
+      <c r="C17" s="91">
         <v>2</v>
       </c>
-      <c r="D17" s="101" t="s">
+      <c r="D17" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
+      <c r="E17" s="108"/>
+      <c r="F17" s="108"/>
+      <c r="G17" s="108"/>
       <c r="H17" s="33"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -8283,19 +8285,19 @@
       <c r="CN17" s="46"/>
     </row>
     <row r="18" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C18" s="84">
+      <c r="C18" s="79">
         <v>2.1</v>
       </c>
-      <c r="D18" s="89" t="s">
+      <c r="D18" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="86">
+      <c r="E18" s="81">
         <v>1</v>
       </c>
-      <c r="F18" s="87">
+      <c r="F18" s="82">
         <v>44427</v>
       </c>
-      <c r="G18" s="87">
+      <c r="G18" s="82">
         <v>44433</v>
       </c>
       <c r="H18" s="33"/>
@@ -8316,13 +8318,13 @@
       <c r="W18" s="8"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
-      <c r="Z18" s="107"/>
-      <c r="AA18" s="107"/>
+      <c r="Z18" s="99"/>
+      <c r="AA18" s="99"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="8"/>
-      <c r="AD18" s="107"/>
-      <c r="AE18" s="107"/>
-      <c r="AF18" s="107"/>
+      <c r="AD18" s="99"/>
+      <c r="AE18" s="99"/>
+      <c r="AF18" s="99"/>
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
       <c r="AI18" s="8"/>
@@ -8385,19 +8387,19 @@
       <c r="CN18" s="46"/>
     </row>
     <row r="19" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C19" s="84">
+      <c r="C19" s="79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D19" s="89" t="s">
+      <c r="D19" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="E19" s="86">
+      <c r="E19" s="81">
         <v>1</v>
       </c>
-      <c r="F19" s="87">
+      <c r="F19" s="82">
         <v>44427</v>
       </c>
-      <c r="G19" s="87">
+      <c r="G19" s="82">
         <v>44433</v>
       </c>
       <c r="H19" s="33"/>
@@ -8418,13 +8420,13 @@
       <c r="W19" s="8"/>
       <c r="X19" s="8"/>
       <c r="Y19" s="8"/>
-      <c r="Z19" s="107"/>
-      <c r="AA19" s="107"/>
+      <c r="Z19" s="99"/>
+      <c r="AA19" s="99"/>
       <c r="AB19" s="8"/>
       <c r="AC19" s="8"/>
-      <c r="AD19" s="107"/>
-      <c r="AE19" s="107"/>
-      <c r="AF19" s="107"/>
+      <c r="AD19" s="99"/>
+      <c r="AE19" s="99"/>
+      <c r="AF19" s="99"/>
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
       <c r="AI19" s="8"/>
@@ -8487,19 +8489,19 @@
       <c r="CN19" s="46"/>
     </row>
     <row r="20" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C20" s="84">
+      <c r="C20" s="79">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D20" s="89" t="s">
+      <c r="D20" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="86">
+      <c r="E20" s="81">
         <v>1</v>
       </c>
-      <c r="F20" s="87">
+      <c r="F20" s="82">
         <v>44427</v>
       </c>
-      <c r="G20" s="87">
+      <c r="G20" s="82">
         <v>44433</v>
       </c>
       <c r="H20" s="33"/>
@@ -8520,13 +8522,13 @@
       <c r="W20" s="8"/>
       <c r="X20" s="8"/>
       <c r="Y20" s="8"/>
-      <c r="Z20" s="107"/>
-      <c r="AA20" s="107"/>
+      <c r="Z20" s="99"/>
+      <c r="AA20" s="99"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="8"/>
-      <c r="AD20" s="107"/>
-      <c r="AE20" s="107"/>
-      <c r="AF20" s="107"/>
+      <c r="AD20" s="99"/>
+      <c r="AE20" s="99"/>
+      <c r="AF20" s="99"/>
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
       <c r="AI20" s="8"/>
@@ -8589,19 +8591,19 @@
       <c r="CN20" s="46"/>
     </row>
     <row r="21" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C21" s="84">
+      <c r="C21" s="79">
         <v>2.4</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="84" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="86">
+      <c r="E21" s="81">
         <v>1</v>
       </c>
-      <c r="F21" s="87">
+      <c r="F21" s="82">
         <v>44427</v>
       </c>
-      <c r="G21" s="87">
+      <c r="G21" s="82">
         <v>44433</v>
       </c>
       <c r="H21" s="33"/>
@@ -8622,13 +8624,13 @@
       <c r="W21" s="8"/>
       <c r="X21" s="8"/>
       <c r="Y21" s="8"/>
-      <c r="Z21" s="107"/>
-      <c r="AA21" s="107"/>
+      <c r="Z21" s="99"/>
+      <c r="AA21" s="99"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
-      <c r="AD21" s="107"/>
-      <c r="AE21" s="107"/>
-      <c r="AF21" s="107"/>
+      <c r="AD21" s="99"/>
+      <c r="AE21" s="99"/>
+      <c r="AF21" s="99"/>
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
@@ -8691,19 +8693,19 @@
       <c r="CN21" s="46"/>
     </row>
     <row r="22" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C22" s="84">
+      <c r="C22" s="79">
         <v>2.5</v>
       </c>
-      <c r="D22" s="89" t="s">
+      <c r="D22" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="86">
+      <c r="E22" s="81">
         <v>1</v>
       </c>
-      <c r="F22" s="87">
+      <c r="F22" s="82">
         <v>44428</v>
       </c>
-      <c r="G22" s="87">
+      <c r="G22" s="82">
         <v>44435</v>
       </c>
       <c r="H22" s="33"/>
@@ -8728,11 +8730,11 @@
       <c r="AA22" s="47"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
-      <c r="AD22" s="107"/>
-      <c r="AE22" s="107"/>
-      <c r="AF22" s="107"/>
-      <c r="AG22" s="107"/>
-      <c r="AH22" s="107"/>
+      <c r="AD22" s="99"/>
+      <c r="AE22" s="99"/>
+      <c r="AF22" s="99"/>
+      <c r="AG22" s="99"/>
+      <c r="AH22" s="99"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8"/>
       <c r="AK22" s="8"/>
@@ -8793,19 +8795,19 @@
       <c r="CN22" s="46"/>
     </row>
     <row r="23" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C23" s="84">
+      <c r="C23" s="79">
         <v>2.6</v>
       </c>
-      <c r="D23" s="89" t="s">
+      <c r="D23" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="86">
+      <c r="E23" s="81">
         <v>1</v>
       </c>
-      <c r="F23" s="87">
+      <c r="F23" s="82">
         <v>44428</v>
       </c>
-      <c r="G23" s="87">
+      <c r="G23" s="82">
         <v>44435</v>
       </c>
       <c r="H23" s="33"/>
@@ -8830,11 +8832,11 @@
       <c r="AA23" s="47"/>
       <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
-      <c r="AD23" s="107"/>
-      <c r="AE23" s="107"/>
-      <c r="AF23" s="107"/>
-      <c r="AG23" s="107"/>
-      <c r="AH23" s="107"/>
+      <c r="AD23" s="99"/>
+      <c r="AE23" s="99"/>
+      <c r="AF23" s="99"/>
+      <c r="AG23" s="99"/>
+      <c r="AH23" s="99"/>
       <c r="AI23" s="8"/>
       <c r="AJ23" s="8"/>
       <c r="AK23" s="8"/>
@@ -8895,19 +8897,19 @@
       <c r="CN23" s="46"/>
     </row>
     <row r="24" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C24" s="84">
+      <c r="C24" s="79">
         <v>2.7</v>
       </c>
-      <c r="D24" s="89" t="s">
+      <c r="D24" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="86">
+      <c r="E24" s="81">
         <v>1</v>
       </c>
-      <c r="F24" s="87">
+      <c r="F24" s="82">
         <v>44428</v>
       </c>
-      <c r="G24" s="87">
+      <c r="G24" s="82">
         <v>44435</v>
       </c>
       <c r="H24" s="33"/>
@@ -8932,11 +8934,11 @@
       <c r="AA24" s="47"/>
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
-      <c r="AD24" s="107"/>
-      <c r="AE24" s="107"/>
-      <c r="AF24" s="107"/>
-      <c r="AG24" s="107"/>
-      <c r="AH24" s="107"/>
+      <c r="AD24" s="99"/>
+      <c r="AE24" s="99"/>
+      <c r="AF24" s="99"/>
+      <c r="AG24" s="99"/>
+      <c r="AH24" s="99"/>
       <c r="AI24" s="8"/>
       <c r="AJ24" s="8"/>
       <c r="AK24" s="8"/>
@@ -8998,13 +9000,13 @@
     </row>
     <row r="25" spans="2:92" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B25" s="6"/>
-      <c r="C25" s="102"/>
-      <c r="D25" s="96" t="s">
+      <c r="C25" s="95"/>
+      <c r="D25" s="107" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
+      <c r="E25" s="107"/>
+      <c r="F25" s="107"/>
+      <c r="G25" s="107"/>
       <c r="H25" s="30"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
@@ -9093,15 +9095,15 @@
     </row>
     <row r="26" spans="2:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
-      <c r="C26" s="97">
+      <c r="C26" s="91">
         <v>1</v>
       </c>
-      <c r="D26" s="98" t="s">
+      <c r="D26" s="92" t="s">
         <v>177</v>
       </c>
-      <c r="E26" s="98"/>
-      <c r="F26" s="99"/>
-      <c r="G26" s="99"/>
+      <c r="E26" s="92"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
       <c r="H26" s="30"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -9189,17 +9191,21 @@
       <c r="CN26" s="46"/>
     </row>
     <row r="27" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C27" s="91">
+      <c r="C27" s="86">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D27" s="89" t="s">
+      <c r="D27" s="84" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="86">
-        <v>0</v>
-      </c>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="E27" s="81">
+        <v>1</v>
+      </c>
+      <c r="F27" s="82">
+        <v>44438</v>
+      </c>
+      <c r="G27" s="82">
+        <v>44440</v>
+      </c>
       <c r="H27" s="47"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
@@ -9229,10 +9235,10 @@
       <c r="AH27" s="8"/>
       <c r="AI27" s="8"/>
       <c r="AJ27" s="8"/>
-      <c r="AK27" s="109"/>
-      <c r="AL27" s="107"/>
-      <c r="AM27" s="107"/>
-      <c r="AN27" s="107"/>
+      <c r="AK27" s="101"/>
+      <c r="AL27" s="99"/>
+      <c r="AM27" s="99"/>
+      <c r="AN27" s="47"/>
       <c r="AO27" s="8"/>
       <c r="AP27" s="8"/>
       <c r="AQ27" s="8"/>
@@ -9288,15 +9294,15 @@
     </row>
     <row r="28" spans="2:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="7"/>
-      <c r="C28" s="97">
+      <c r="C28" s="91">
         <v>2</v>
       </c>
-      <c r="D28" s="98" t="s">
+      <c r="D28" s="92" t="s">
         <v>95</v>
       </c>
-      <c r="E28" s="98"/>
-      <c r="F28" s="99"/>
-      <c r="G28" s="99"/>
+      <c r="E28" s="92"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="93"/>
       <c r="H28" s="30"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
@@ -9380,17 +9386,19 @@
       <c r="CN28" s="46"/>
     </row>
     <row r="29" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C29" s="84">
+      <c r="C29" s="79">
         <v>2.1</v>
       </c>
-      <c r="D29" s="90" t="s">
+      <c r="D29" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="E29" s="86">
+      <c r="E29" s="81">
         <v>0</v>
       </c>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
+      <c r="F29" s="82">
+        <v>44440</v>
+      </c>
+      <c r="G29" s="82"/>
       <c r="H29" s="34"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
@@ -9422,13 +9430,13 @@
       <c r="AJ29" s="8"/>
       <c r="AK29" s="47"/>
       <c r="AL29" s="47"/>
-      <c r="AM29" s="107"/>
-      <c r="AN29" s="107"/>
-      <c r="AO29" s="107"/>
+      <c r="AM29" s="99"/>
+      <c r="AN29" s="99"/>
+      <c r="AO29" s="99"/>
       <c r="AP29" s="8"/>
       <c r="AQ29" s="8"/>
-      <c r="AR29" s="107"/>
-      <c r="AS29" s="107"/>
+      <c r="AR29" s="99"/>
+      <c r="AS29" s="99"/>
       <c r="AT29" s="8"/>
       <c r="AU29" s="8"/>
       <c r="AV29" s="8"/>
@@ -9478,17 +9486,19 @@
       <c r="CN29" s="46"/>
     </row>
     <row r="30" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C30" s="91">
+      <c r="C30" s="86">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D30" s="90" t="s">
+      <c r="D30" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="E30" s="86">
+      <c r="E30" s="81">
         <v>0</v>
       </c>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
+      <c r="F30" s="82">
+        <v>44440</v>
+      </c>
+      <c r="G30" s="82"/>
       <c r="H30" s="34"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
@@ -9520,13 +9530,13 @@
       <c r="AJ30" s="8"/>
       <c r="AK30" s="47"/>
       <c r="AL30" s="47"/>
-      <c r="AM30" s="107"/>
-      <c r="AN30" s="107"/>
-      <c r="AO30" s="107"/>
+      <c r="AM30" s="99"/>
+      <c r="AN30" s="99"/>
+      <c r="AO30" s="99"/>
       <c r="AP30" s="8"/>
       <c r="AQ30" s="8"/>
-      <c r="AR30" s="107"/>
-      <c r="AS30" s="107"/>
+      <c r="AR30" s="99"/>
+      <c r="AS30" s="99"/>
       <c r="AT30" s="8"/>
       <c r="AU30" s="8"/>
       <c r="AV30" s="8"/>
@@ -9576,17 +9586,19 @@
       <c r="CN30" s="46"/>
     </row>
     <row r="31" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C31" s="84">
+      <c r="C31" s="79">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D31" s="90" t="s">
+      <c r="D31" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="E31" s="86">
+      <c r="E31" s="81">
         <v>0</v>
       </c>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
+      <c r="F31" s="82">
+        <v>44440</v>
+      </c>
+      <c r="G31" s="82"/>
       <c r="H31" s="34"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
@@ -9618,13 +9630,13 @@
       <c r="AJ31" s="8"/>
       <c r="AK31" s="47"/>
       <c r="AL31" s="47"/>
-      <c r="AM31" s="107"/>
-      <c r="AN31" s="107"/>
-      <c r="AO31" s="107"/>
+      <c r="AM31" s="99"/>
+      <c r="AN31" s="99"/>
+      <c r="AO31" s="99"/>
       <c r="AP31" s="8"/>
       <c r="AQ31" s="8"/>
-      <c r="AR31" s="107"/>
-      <c r="AS31" s="107"/>
+      <c r="AR31" s="99"/>
+      <c r="AS31" s="99"/>
       <c r="AT31" s="8"/>
       <c r="AU31" s="8"/>
       <c r="AV31" s="8"/>
@@ -9674,17 +9686,19 @@
       <c r="CN31" s="46"/>
     </row>
     <row r="32" spans="2:92" x14ac:dyDescent="0.25">
-      <c r="C32" s="91">
+      <c r="C32" s="86">
         <v>2.4</v>
       </c>
-      <c r="D32" s="90" t="s">
+      <c r="D32" s="85" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="86">
+      <c r="E32" s="81">
         <v>0</v>
       </c>
-      <c r="F32" s="87"/>
-      <c r="G32" s="87"/>
+      <c r="F32" s="82">
+        <v>44440</v>
+      </c>
+      <c r="G32" s="82"/>
       <c r="H32" s="34"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
@@ -9716,13 +9730,13 @@
       <c r="AJ32" s="8"/>
       <c r="AK32" s="47"/>
       <c r="AL32" s="47"/>
-      <c r="AM32" s="107"/>
-      <c r="AN32" s="107"/>
-      <c r="AO32" s="107"/>
+      <c r="AM32" s="99"/>
+      <c r="AN32" s="99"/>
+      <c r="AO32" s="99"/>
       <c r="AP32" s="8"/>
       <c r="AQ32" s="8"/>
-      <c r="AR32" s="107"/>
-      <c r="AS32" s="107"/>
+      <c r="AR32" s="99"/>
+      <c r="AS32" s="99"/>
       <c r="AT32" s="8"/>
       <c r="AU32" s="8"/>
       <c r="AV32" s="8"/>
@@ -9772,17 +9786,19 @@
       <c r="CN32" s="46"/>
     </row>
     <row r="33" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C33" s="84">
+      <c r="C33" s="79">
         <v>2.5</v>
       </c>
-      <c r="D33" s="90" t="s">
+      <c r="D33" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="E33" s="86">
+      <c r="E33" s="81">
         <v>0</v>
       </c>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
+      <c r="F33" s="82">
+        <v>44440</v>
+      </c>
+      <c r="G33" s="82"/>
       <c r="H33" s="34"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
@@ -9814,13 +9830,13 @@
       <c r="AJ33" s="8"/>
       <c r="AK33" s="47"/>
       <c r="AL33" s="47"/>
-      <c r="AM33" s="107"/>
-      <c r="AN33" s="107"/>
-      <c r="AO33" s="107"/>
+      <c r="AM33" s="99"/>
+      <c r="AN33" s="99"/>
+      <c r="AO33" s="99"/>
       <c r="AP33" s="8"/>
       <c r="AQ33" s="8"/>
-      <c r="AR33" s="107"/>
-      <c r="AS33" s="107"/>
+      <c r="AR33" s="99"/>
+      <c r="AS33" s="99"/>
       <c r="AT33" s="8"/>
       <c r="AU33" s="8"/>
       <c r="AV33" s="8"/>
@@ -9870,15 +9886,15 @@
       <c r="CN33" s="46"/>
     </row>
     <row r="34" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C34" s="97">
+      <c r="C34" s="91">
         <v>3</v>
       </c>
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="98"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="99"/>
+      <c r="E34" s="92"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
       <c r="H34" s="34"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
@@ -9966,17 +9982,17 @@
       <c r="CN34" s="46"/>
     </row>
     <row r="35" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C35" s="92">
+      <c r="C35" s="87">
         <v>3.1</v>
       </c>
-      <c r="D35" s="90" t="s">
+      <c r="D35" s="85" t="s">
         <v>101</v>
       </c>
-      <c r="E35" s="86">
+      <c r="E35" s="81">
         <v>0</v>
       </c>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
       <c r="H35" s="34"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
@@ -10009,15 +10025,15 @@
       <c r="AK35" s="8"/>
       <c r="AL35" s="8"/>
       <c r="AM35" s="47"/>
-      <c r="AN35" s="107"/>
-      <c r="AO35" s="107"/>
+      <c r="AN35" s="99"/>
+      <c r="AO35" s="99"/>
       <c r="AP35" s="8"/>
       <c r="AQ35" s="8"/>
-      <c r="AR35" s="107"/>
-      <c r="AS35" s="107"/>
-      <c r="AT35" s="107"/>
-      <c r="AU35" s="107"/>
-      <c r="AV35" s="107"/>
+      <c r="AR35" s="99"/>
+      <c r="AS35" s="99"/>
+      <c r="AT35" s="99"/>
+      <c r="AU35" s="99"/>
+      <c r="AV35" s="99"/>
       <c r="AW35" s="8"/>
       <c r="AX35" s="8"/>
       <c r="AY35" s="8"/>
@@ -10064,17 +10080,17 @@
       <c r="CN35" s="46"/>
     </row>
     <row r="36" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C36" s="93">
+      <c r="C36" s="88">
         <v>3.2</v>
       </c>
-      <c r="D36" s="90" t="s">
+      <c r="D36" s="85" t="s">
         <v>111</v>
       </c>
-      <c r="E36" s="86">
+      <c r="E36" s="81">
         <v>0</v>
       </c>
-      <c r="F36" s="87"/>
-      <c r="G36" s="87"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
       <c r="H36" s="34"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
@@ -10107,15 +10123,15 @@
       <c r="AK36" s="8"/>
       <c r="AL36" s="8"/>
       <c r="AM36" s="47"/>
-      <c r="AN36" s="107"/>
-      <c r="AO36" s="107"/>
+      <c r="AN36" s="99"/>
+      <c r="AO36" s="99"/>
       <c r="AP36" s="8"/>
       <c r="AQ36" s="8"/>
-      <c r="AR36" s="107"/>
-      <c r="AS36" s="107"/>
-      <c r="AT36" s="107"/>
-      <c r="AU36" s="107"/>
-      <c r="AV36" s="107"/>
+      <c r="AR36" s="99"/>
+      <c r="AS36" s="99"/>
+      <c r="AT36" s="99"/>
+      <c r="AU36" s="99"/>
+      <c r="AV36" s="99"/>
       <c r="AW36" s="8"/>
       <c r="AX36" s="8"/>
       <c r="AY36" s="8"/>
@@ -10162,17 +10178,17 @@
       <c r="CN36" s="46"/>
     </row>
     <row r="37" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C37" s="93" t="s">
+      <c r="C37" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="D37" s="90" t="s">
+      <c r="D37" s="85" t="s">
         <v>112</v>
       </c>
-      <c r="E37" s="86">
+      <c r="E37" s="81">
         <v>0</v>
       </c>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
       <c r="H37" s="34"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
@@ -10205,15 +10221,15 @@
       <c r="AK37" s="8"/>
       <c r="AL37" s="8"/>
       <c r="AM37" s="47"/>
-      <c r="AN37" s="107"/>
-      <c r="AO37" s="107"/>
+      <c r="AN37" s="99"/>
+      <c r="AO37" s="99"/>
       <c r="AP37" s="8"/>
       <c r="AQ37" s="8"/>
-      <c r="AR37" s="107"/>
-      <c r="AS37" s="107"/>
-      <c r="AT37" s="107"/>
-      <c r="AU37" s="107"/>
-      <c r="AV37" s="107"/>
+      <c r="AR37" s="99"/>
+      <c r="AS37" s="99"/>
+      <c r="AT37" s="99"/>
+      <c r="AU37" s="99"/>
+      <c r="AV37" s="99"/>
       <c r="AW37" s="8"/>
       <c r="AX37" s="8"/>
       <c r="AY37" s="8"/>
@@ -10260,17 +10276,17 @@
       <c r="CN37" s="46"/>
     </row>
     <row r="38" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C38" s="93" t="s">
+      <c r="C38" s="88" t="s">
         <v>179</v>
       </c>
-      <c r="D38" s="90" t="s">
+      <c r="D38" s="85" t="s">
         <v>103</v>
       </c>
-      <c r="E38" s="86">
+      <c r="E38" s="81">
         <v>0</v>
       </c>
-      <c r="F38" s="87"/>
-      <c r="G38" s="87"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
       <c r="H38" s="34"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
@@ -10303,15 +10319,15 @@
       <c r="AK38" s="8"/>
       <c r="AL38" s="8"/>
       <c r="AM38" s="47"/>
-      <c r="AN38" s="107"/>
-      <c r="AO38" s="107"/>
+      <c r="AN38" s="99"/>
+      <c r="AO38" s="99"/>
       <c r="AP38" s="8"/>
       <c r="AQ38" s="8"/>
-      <c r="AR38" s="107"/>
-      <c r="AS38" s="107"/>
-      <c r="AT38" s="107"/>
-      <c r="AU38" s="107"/>
-      <c r="AV38" s="107"/>
+      <c r="AR38" s="99"/>
+      <c r="AS38" s="99"/>
+      <c r="AT38" s="99"/>
+      <c r="AU38" s="99"/>
+      <c r="AV38" s="99"/>
       <c r="AW38" s="8"/>
       <c r="AX38" s="8"/>
       <c r="AY38" s="8"/>
@@ -10358,17 +10374,17 @@
       <c r="CN38" s="46"/>
     </row>
     <row r="39" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C39" s="84">
+      <c r="C39" s="79">
         <v>3.3</v>
       </c>
-      <c r="D39" s="90" t="s">
+      <c r="D39" s="85" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="86">
+      <c r="E39" s="81">
         <v>0</v>
       </c>
-      <c r="F39" s="87"/>
-      <c r="G39" s="87"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
       <c r="H39" s="34"/>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -10401,15 +10417,15 @@
       <c r="AK39" s="8"/>
       <c r="AL39" s="8"/>
       <c r="AM39" s="8"/>
-      <c r="AN39" s="107"/>
-      <c r="AO39" s="107"/>
+      <c r="AN39" s="99"/>
+      <c r="AO39" s="99"/>
       <c r="AP39" s="8"/>
       <c r="AQ39" s="8"/>
-      <c r="AR39" s="107"/>
-      <c r="AS39" s="107"/>
-      <c r="AT39" s="107"/>
-      <c r="AU39" s="107"/>
-      <c r="AV39" s="107"/>
+      <c r="AR39" s="99"/>
+      <c r="AS39" s="99"/>
+      <c r="AT39" s="99"/>
+      <c r="AU39" s="99"/>
+      <c r="AV39" s="99"/>
       <c r="AW39" s="8"/>
       <c r="AX39" s="8"/>
       <c r="AY39" s="8"/>
@@ -10456,17 +10472,17 @@
       <c r="CN39" s="46"/>
     </row>
     <row r="40" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C40" s="84" t="s">
+      <c r="C40" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="D40" s="90" t="s">
+      <c r="D40" s="85" t="s">
         <v>144</v>
       </c>
-      <c r="E40" s="86">
+      <c r="E40" s="81">
         <v>0</v>
       </c>
-      <c r="F40" s="87"/>
-      <c r="G40" s="87"/>
+      <c r="F40" s="82"/>
+      <c r="G40" s="82"/>
       <c r="H40" s="34"/>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
@@ -10499,15 +10515,15 @@
       <c r="AK40" s="8"/>
       <c r="AL40" s="8"/>
       <c r="AM40" s="8"/>
-      <c r="AN40" s="107"/>
-      <c r="AO40" s="107"/>
+      <c r="AN40" s="99"/>
+      <c r="AO40" s="99"/>
       <c r="AP40" s="8"/>
       <c r="AQ40" s="8"/>
-      <c r="AR40" s="107"/>
-      <c r="AS40" s="107"/>
-      <c r="AT40" s="107"/>
-      <c r="AU40" s="107"/>
-      <c r="AV40" s="107"/>
+      <c r="AR40" s="99"/>
+      <c r="AS40" s="99"/>
+      <c r="AT40" s="99"/>
+      <c r="AU40" s="99"/>
+      <c r="AV40" s="99"/>
       <c r="AW40" s="8"/>
       <c r="AX40" s="8"/>
       <c r="AY40" s="8"/>
@@ -10554,17 +10570,17 @@
       <c r="CN40" s="46"/>
     </row>
     <row r="41" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C41" s="84" t="s">
+      <c r="C41" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="D41" s="90" t="s">
+      <c r="D41" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="E41" s="86">
+      <c r="E41" s="81">
         <v>0</v>
       </c>
-      <c r="F41" s="87"/>
-      <c r="G41" s="87"/>
+      <c r="F41" s="82"/>
+      <c r="G41" s="82"/>
       <c r="H41" s="34"/>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
@@ -10597,15 +10613,15 @@
       <c r="AK41" s="8"/>
       <c r="AL41" s="8"/>
       <c r="AM41" s="8"/>
-      <c r="AN41" s="107"/>
-      <c r="AO41" s="107"/>
+      <c r="AN41" s="99"/>
+      <c r="AO41" s="99"/>
       <c r="AP41" s="8"/>
       <c r="AQ41" s="8"/>
-      <c r="AR41" s="107"/>
-      <c r="AS41" s="107"/>
-      <c r="AT41" s="107"/>
-      <c r="AU41" s="107"/>
-      <c r="AV41" s="107"/>
+      <c r="AR41" s="99"/>
+      <c r="AS41" s="99"/>
+      <c r="AT41" s="99"/>
+      <c r="AU41" s="99"/>
+      <c r="AV41" s="99"/>
       <c r="AW41" s="8"/>
       <c r="AX41" s="8"/>
       <c r="AY41" s="8"/>
@@ -10652,17 +10668,17 @@
       <c r="CN41" s="46"/>
     </row>
     <row r="42" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C42" s="84" t="s">
+      <c r="C42" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="90" t="s">
+      <c r="D42" s="85" t="s">
         <v>146</v>
       </c>
-      <c r="E42" s="86">
+      <c r="E42" s="81">
         <v>0</v>
       </c>
-      <c r="F42" s="87"/>
-      <c r="G42" s="87"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
       <c r="H42" s="34"/>
       <c r="I42" s="27"/>
       <c r="J42" s="27"/>
@@ -10695,15 +10711,15 @@
       <c r="AK42" s="8"/>
       <c r="AL42" s="8"/>
       <c r="AM42" s="8"/>
-      <c r="AN42" s="107"/>
-      <c r="AO42" s="107"/>
+      <c r="AN42" s="99"/>
+      <c r="AO42" s="99"/>
       <c r="AP42" s="8"/>
       <c r="AQ42" s="8"/>
-      <c r="AR42" s="107"/>
-      <c r="AS42" s="107"/>
-      <c r="AT42" s="107"/>
-      <c r="AU42" s="107"/>
-      <c r="AV42" s="107"/>
+      <c r="AR42" s="99"/>
+      <c r="AS42" s="99"/>
+      <c r="AT42" s="99"/>
+      <c r="AU42" s="99"/>
+      <c r="AV42" s="99"/>
       <c r="AW42" s="8"/>
       <c r="AX42" s="8"/>
       <c r="AY42" s="8"/>
@@ -10750,17 +10766,17 @@
       <c r="CN42" s="46"/>
     </row>
     <row r="43" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C43" s="84">
+      <c r="C43" s="79">
         <v>3.4</v>
       </c>
-      <c r="D43" s="90" t="s">
+      <c r="D43" s="85" t="s">
         <v>106</v>
       </c>
-      <c r="E43" s="86">
+      <c r="E43" s="81">
         <v>0</v>
       </c>
-      <c r="F43" s="87"/>
-      <c r="G43" s="87"/>
+      <c r="F43" s="82"/>
+      <c r="G43" s="82"/>
       <c r="H43" s="34"/>
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
@@ -10798,10 +10814,10 @@
       <c r="AP43" s="8"/>
       <c r="AQ43" s="8"/>
       <c r="AR43" s="8"/>
-      <c r="AS43" s="107"/>
-      <c r="AT43" s="107"/>
-      <c r="AU43" s="107"/>
-      <c r="AV43" s="107"/>
+      <c r="AS43" s="99"/>
+      <c r="AT43" s="99"/>
+      <c r="AU43" s="99"/>
+      <c r="AV43" s="99"/>
       <c r="AW43" s="8"/>
       <c r="AX43" s="8"/>
       <c r="AY43" s="8"/>
@@ -10848,17 +10864,17 @@
       <c r="CN43" s="46"/>
     </row>
     <row r="44" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C44" s="84" t="s">
+      <c r="C44" s="79" t="s">
         <v>183</v>
       </c>
-      <c r="D44" s="90" t="s">
+      <c r="D44" s="85" t="s">
         <v>105</v>
       </c>
-      <c r="E44" s="86">
+      <c r="E44" s="81">
         <v>0</v>
       </c>
-      <c r="F44" s="87"/>
-      <c r="G44" s="87"/>
+      <c r="F44" s="82"/>
+      <c r="G44" s="82"/>
       <c r="H44" s="34"/>
       <c r="I44" s="27"/>
       <c r="J44" s="27"/>
@@ -10896,10 +10912,10 @@
       <c r="AP44" s="8"/>
       <c r="AQ44" s="8"/>
       <c r="AR44" s="8"/>
-      <c r="AS44" s="107"/>
-      <c r="AT44" s="107"/>
-      <c r="AU44" s="107"/>
-      <c r="AV44" s="107"/>
+      <c r="AS44" s="99"/>
+      <c r="AT44" s="99"/>
+      <c r="AU44" s="99"/>
+      <c r="AV44" s="99"/>
       <c r="AW44" s="8"/>
       <c r="AX44" s="8"/>
       <c r="AY44" s="8"/>
@@ -10946,17 +10962,17 @@
       <c r="CN44" s="46"/>
     </row>
     <row r="45" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C45" s="94">
+      <c r="C45" s="89">
         <v>3.5</v>
       </c>
-      <c r="D45" s="90" t="s">
+      <c r="D45" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="E45" s="86">
+      <c r="E45" s="81">
         <v>0</v>
       </c>
-      <c r="F45" s="87"/>
-      <c r="G45" s="87"/>
+      <c r="F45" s="82"/>
+      <c r="G45" s="82"/>
       <c r="H45" s="34"/>
       <c r="I45" s="27"/>
       <c r="J45" s="27"/>
@@ -10994,10 +11010,10 @@
       <c r="AP45" s="8"/>
       <c r="AQ45" s="8"/>
       <c r="AR45" s="8"/>
-      <c r="AS45" s="107"/>
-      <c r="AT45" s="107"/>
-      <c r="AU45" s="107"/>
-      <c r="AV45" s="107"/>
+      <c r="AS45" s="99"/>
+      <c r="AT45" s="99"/>
+      <c r="AU45" s="99"/>
+      <c r="AV45" s="99"/>
       <c r="AW45" s="8"/>
       <c r="AX45" s="8"/>
       <c r="AY45" s="8"/>
@@ -11044,15 +11060,15 @@
       <c r="CN45" s="46"/>
     </row>
     <row r="46" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C46" s="97">
+      <c r="C46" s="91">
         <v>4</v>
       </c>
-      <c r="D46" s="101" t="s">
+      <c r="D46" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="101"/>
-      <c r="F46" s="101"/>
-      <c r="G46" s="101"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
       <c r="H46" s="34"/>
       <c r="I46" s="27"/>
       <c r="J46" s="27"/>
@@ -11140,17 +11156,17 @@
       <c r="CN46" s="46"/>
     </row>
     <row r="47" spans="3:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="84">
+      <c r="C47" s="79">
         <v>4.0999999999999996</v>
       </c>
-      <c r="D47" s="95" t="s">
+      <c r="D47" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="E47" s="86">
+      <c r="E47" s="81">
         <v>0</v>
       </c>
-      <c r="F47" s="87"/>
-      <c r="G47" s="87"/>
+      <c r="F47" s="82"/>
+      <c r="G47" s="82"/>
       <c r="H47" s="34"/>
       <c r="I47" s="27"/>
       <c r="J47" s="27"/>
@@ -11189,9 +11205,9 @@
       <c r="AQ47" s="8"/>
       <c r="AR47" s="8"/>
       <c r="AS47" s="8"/>
-      <c r="AT47" s="107"/>
-      <c r="AU47" s="107"/>
-      <c r="AV47" s="107"/>
+      <c r="AT47" s="99"/>
+      <c r="AU47" s="99"/>
+      <c r="AV47" s="99"/>
       <c r="AW47" s="8"/>
       <c r="AX47" s="8"/>
       <c r="AY47" s="8"/>
@@ -11238,13 +11254,13 @@
       <c r="CN47" s="46"/>
     </row>
     <row r="48" spans="3:92" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C48" s="103"/>
-      <c r="D48" s="96" t="s">
+      <c r="C48" s="96"/>
+      <c r="D48" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="96"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="96"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
       <c r="H48" s="30"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
@@ -11332,15 +11348,15 @@
       <c r="CN48" s="46"/>
     </row>
     <row r="49" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C49" s="97">
+      <c r="C49" s="91">
         <v>1</v>
       </c>
-      <c r="D49" s="98" t="s">
+      <c r="D49" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="98"/>
-      <c r="F49" s="99"/>
-      <c r="G49" s="99"/>
+      <c r="E49" s="92"/>
+      <c r="F49" s="93"/>
+      <c r="G49" s="93"/>
       <c r="H49" s="30"/>
       <c r="I49" s="8"/>
       <c r="J49" s="8"/>
@@ -11428,17 +11444,17 @@
       <c r="CN49" s="46"/>
     </row>
     <row r="50" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C50" s="84">
+      <c r="C50" s="79">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D50" s="90" t="s">
+      <c r="D50" s="85" t="s">
         <v>113</v>
       </c>
-      <c r="E50" s="86">
+      <c r="E50" s="81">
         <v>0</v>
       </c>
-      <c r="F50" s="87"/>
-      <c r="G50" s="87"/>
+      <c r="F50" s="82"/>
+      <c r="G50" s="82"/>
       <c r="H50" s="34"/>
       <c r="I50" s="27"/>
       <c r="J50" s="27"/>
@@ -11482,10 +11498,10 @@
       <c r="AV50" s="8"/>
       <c r="AW50" s="8"/>
       <c r="AX50" s="8"/>
-      <c r="AY50" s="107"/>
-      <c r="AZ50" s="107"/>
-      <c r="BA50" s="107"/>
-      <c r="BB50" s="107"/>
+      <c r="AY50" s="99"/>
+      <c r="AZ50" s="99"/>
+      <c r="BA50" s="99"/>
+      <c r="BB50" s="99"/>
       <c r="BC50" s="8"/>
       <c r="BD50" s="8"/>
       <c r="BE50" s="8"/>
@@ -11526,17 +11542,17 @@
       <c r="CN50" s="46"/>
     </row>
     <row r="51" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C51" s="91" t="s">
+      <c r="C51" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="D51" s="90" t="s">
+      <c r="D51" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="E51" s="86">
+      <c r="E51" s="81">
         <v>0</v>
       </c>
-      <c r="F51" s="87"/>
-      <c r="G51" s="87"/>
+      <c r="F51" s="82"/>
+      <c r="G51" s="82"/>
       <c r="H51" s="34"/>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
@@ -11580,10 +11596,10 @@
       <c r="AV51" s="8"/>
       <c r="AW51" s="8"/>
       <c r="AX51" s="8"/>
-      <c r="AY51" s="107"/>
-      <c r="AZ51" s="107"/>
-      <c r="BA51" s="107"/>
-      <c r="BB51" s="107"/>
+      <c r="AY51" s="99"/>
+      <c r="AZ51" s="99"/>
+      <c r="BA51" s="99"/>
+      <c r="BB51" s="99"/>
       <c r="BC51" s="8"/>
       <c r="BD51" s="8"/>
       <c r="BE51" s="8"/>
@@ -11624,17 +11640,17 @@
       <c r="CN51" s="46"/>
     </row>
     <row r="52" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C52" s="91" t="s">
+      <c r="C52" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="D52" s="90" t="s">
+      <c r="D52" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="86">
+      <c r="E52" s="81">
         <v>0</v>
       </c>
-      <c r="F52" s="87"/>
-      <c r="G52" s="87"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
       <c r="H52" s="34"/>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
@@ -11678,10 +11694,10 @@
       <c r="AV52" s="8"/>
       <c r="AW52" s="8"/>
       <c r="AX52" s="8"/>
-      <c r="AY52" s="107"/>
-      <c r="AZ52" s="107"/>
-      <c r="BA52" s="107"/>
-      <c r="BB52" s="107"/>
+      <c r="AY52" s="99"/>
+      <c r="AZ52" s="99"/>
+      <c r="BA52" s="99"/>
+      <c r="BB52" s="99"/>
       <c r="BC52" s="8"/>
       <c r="BD52" s="8"/>
       <c r="BE52" s="8"/>
@@ -11722,15 +11738,15 @@
       <c r="CN52" s="46"/>
     </row>
     <row r="53" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C53" s="97">
+      <c r="C53" s="91">
         <v>2</v>
       </c>
-      <c r="D53" s="98" t="s">
+      <c r="D53" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="E53" s="98"/>
-      <c r="F53" s="99"/>
-      <c r="G53" s="99"/>
+      <c r="E53" s="92"/>
+      <c r="F53" s="93"/>
+      <c r="G53" s="93"/>
       <c r="H53" s="34"/>
       <c r="I53" s="27"/>
       <c r="J53" s="27"/>
@@ -11818,17 +11834,17 @@
       <c r="CN53" s="46"/>
     </row>
     <row r="54" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C54" s="84">
+      <c r="C54" s="79">
         <v>2.1</v>
       </c>
-      <c r="D54" s="89" t="s">
+      <c r="D54" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="E54" s="86">
+      <c r="E54" s="81">
         <v>0</v>
       </c>
-      <c r="F54" s="87"/>
-      <c r="G54" s="87"/>
+      <c r="F54" s="82"/>
+      <c r="G54" s="82"/>
       <c r="H54" s="33"/>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
@@ -11874,13 +11890,13 @@
       <c r="AX54" s="8"/>
       <c r="AY54" s="8"/>
       <c r="AZ54" s="8"/>
-      <c r="BA54" s="107"/>
-      <c r="BB54" s="107"/>
-      <c r="BC54" s="107"/>
+      <c r="BA54" s="99"/>
+      <c r="BB54" s="99"/>
+      <c r="BC54" s="99"/>
       <c r="BD54" s="8"/>
       <c r="BE54" s="8"/>
-      <c r="BF54" s="107"/>
-      <c r="BG54" s="107"/>
+      <c r="BF54" s="99"/>
+      <c r="BG54" s="99"/>
       <c r="BH54" s="8"/>
       <c r="BI54" s="8"/>
       <c r="BJ54" s="8"/>
@@ -11916,17 +11932,17 @@
       <c r="CN54" s="46"/>
     </row>
     <row r="55" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C55" s="91" t="s">
+      <c r="C55" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="89" t="s">
+      <c r="D55" s="84" t="s">
         <v>147</v>
       </c>
-      <c r="E55" s="86">
+      <c r="E55" s="81">
         <v>0</v>
       </c>
-      <c r="F55" s="87"/>
-      <c r="G55" s="87"/>
+      <c r="F55" s="82"/>
+      <c r="G55" s="82"/>
       <c r="H55" s="33"/>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
@@ -11972,13 +11988,13 @@
       <c r="AX55" s="8"/>
       <c r="AY55" s="8"/>
       <c r="AZ55" s="8"/>
-      <c r="BA55" s="107"/>
-      <c r="BB55" s="107"/>
-      <c r="BC55" s="107"/>
+      <c r="BA55" s="99"/>
+      <c r="BB55" s="99"/>
+      <c r="BC55" s="99"/>
       <c r="BD55" s="8"/>
       <c r="BE55" s="8"/>
-      <c r="BF55" s="107"/>
-      <c r="BG55" s="107"/>
+      <c r="BF55" s="99"/>
+      <c r="BG55" s="99"/>
       <c r="BH55" s="8"/>
       <c r="BI55" s="8"/>
       <c r="BJ55" s="8"/>
@@ -12014,17 +12030,17 @@
       <c r="CN55" s="46"/>
     </row>
     <row r="56" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C56" s="91">
+      <c r="C56" s="86">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D56" s="89" t="s">
+      <c r="D56" s="84" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="86">
+      <c r="E56" s="81">
         <v>0</v>
       </c>
-      <c r="F56" s="87"/>
-      <c r="G56" s="87"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
       <c r="H56" s="33"/>
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
@@ -12070,13 +12086,13 @@
       <c r="AX56" s="8"/>
       <c r="AY56" s="8"/>
       <c r="AZ56" s="8"/>
-      <c r="BA56" s="107"/>
-      <c r="BB56" s="107"/>
-      <c r="BC56" s="107"/>
+      <c r="BA56" s="99"/>
+      <c r="BB56" s="99"/>
+      <c r="BC56" s="99"/>
       <c r="BD56" s="8"/>
       <c r="BE56" s="8"/>
-      <c r="BF56" s="107"/>
-      <c r="BG56" s="107"/>
+      <c r="BF56" s="99"/>
+      <c r="BG56" s="99"/>
       <c r="BH56" s="8"/>
       <c r="BI56" s="8"/>
       <c r="BJ56" s="8"/>
@@ -12112,17 +12128,17 @@
       <c r="CN56" s="46"/>
     </row>
     <row r="57" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C57" s="91" t="s">
+      <c r="C57" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="89" t="s">
+      <c r="D57" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="E57" s="86">
+      <c r="E57" s="81">
         <v>0</v>
       </c>
-      <c r="F57" s="87"/>
-      <c r="G57" s="87"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
       <c r="H57" s="33"/>
       <c r="I57" s="27"/>
       <c r="J57" s="27"/>
@@ -12168,13 +12184,13 @@
       <c r="AX57" s="8"/>
       <c r="AY57" s="8"/>
       <c r="AZ57" s="8"/>
-      <c r="BA57" s="107"/>
-      <c r="BB57" s="107"/>
-      <c r="BC57" s="107"/>
+      <c r="BA57" s="99"/>
+      <c r="BB57" s="99"/>
+      <c r="BC57" s="99"/>
       <c r="BD57" s="8"/>
       <c r="BE57" s="8"/>
-      <c r="BF57" s="107"/>
-      <c r="BG57" s="107"/>
+      <c r="BF57" s="99"/>
+      <c r="BG57" s="99"/>
       <c r="BH57" s="8"/>
       <c r="BI57" s="8"/>
       <c r="BJ57" s="8"/>
@@ -12210,17 +12226,17 @@
       <c r="CN57" s="46"/>
     </row>
     <row r="58" spans="3:92" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" s="91">
+      <c r="C58" s="86">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D58" s="89" t="s">
+      <c r="D58" s="84" t="s">
         <v>119</v>
       </c>
-      <c r="E58" s="86">
+      <c r="E58" s="81">
         <v>0</v>
       </c>
-      <c r="F58" s="87"/>
-      <c r="G58" s="87"/>
+      <c r="F58" s="82"/>
+      <c r="G58" s="82"/>
       <c r="H58" s="33"/>
       <c r="I58" s="27"/>
       <c r="J58" s="27"/>
@@ -12271,11 +12287,11 @@
       <c r="BC58" s="8"/>
       <c r="BD58" s="8"/>
       <c r="BE58" s="8"/>
-      <c r="BF58" s="107"/>
-      <c r="BG58" s="107"/>
-      <c r="BH58" s="107"/>
-      <c r="BI58" s="107"/>
-      <c r="BJ58" s="107"/>
+      <c r="BF58" s="99"/>
+      <c r="BG58" s="99"/>
+      <c r="BH58" s="99"/>
+      <c r="BI58" s="99"/>
+      <c r="BJ58" s="99"/>
       <c r="BK58" s="8"/>
       <c r="BL58" s="8"/>
       <c r="BM58" s="8"/>
@@ -12308,17 +12324,17 @@
       <c r="CN58" s="46"/>
     </row>
     <row r="59" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C59" s="92">
+      <c r="C59" s="87">
         <v>2.4</v>
       </c>
-      <c r="D59" s="89" t="s">
+      <c r="D59" s="84" t="s">
         <v>121</v>
       </c>
-      <c r="E59" s="86">
+      <c r="E59" s="81">
         <v>0</v>
       </c>
-      <c r="F59" s="87"/>
-      <c r="G59" s="87"/>
+      <c r="F59" s="82"/>
+      <c r="G59" s="82"/>
       <c r="H59" s="33"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
@@ -12369,11 +12385,11 @@
       <c r="BC59" s="8"/>
       <c r="BD59" s="8"/>
       <c r="BE59" s="8"/>
-      <c r="BF59" s="107"/>
-      <c r="BG59" s="107"/>
-      <c r="BH59" s="107"/>
-      <c r="BI59" s="107"/>
-      <c r="BJ59" s="107"/>
+      <c r="BF59" s="99"/>
+      <c r="BG59" s="99"/>
+      <c r="BH59" s="99"/>
+      <c r="BI59" s="99"/>
+      <c r="BJ59" s="99"/>
       <c r="BK59" s="8"/>
       <c r="BL59" s="8"/>
       <c r="BM59" s="8"/>
@@ -12406,17 +12422,17 @@
       <c r="CN59" s="46"/>
     </row>
     <row r="60" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C60" s="84">
+      <c r="C60" s="79">
         <v>2.5</v>
       </c>
-      <c r="D60" s="89" t="s">
+      <c r="D60" s="84" t="s">
         <v>120</v>
       </c>
-      <c r="E60" s="86">
+      <c r="E60" s="81">
         <v>0</v>
       </c>
-      <c r="F60" s="87"/>
-      <c r="G60" s="87"/>
+      <c r="F60" s="82"/>
+      <c r="G60" s="82"/>
       <c r="H60" s="33"/>
       <c r="I60" s="27"/>
       <c r="J60" s="27"/>
@@ -12467,11 +12483,11 @@
       <c r="BC60" s="8"/>
       <c r="BD60" s="8"/>
       <c r="BE60" s="8"/>
-      <c r="BF60" s="107"/>
-      <c r="BG60" s="107"/>
-      <c r="BH60" s="107"/>
-      <c r="BI60" s="107"/>
-      <c r="BJ60" s="107"/>
+      <c r="BF60" s="99"/>
+      <c r="BG60" s="99"/>
+      <c r="BH60" s="99"/>
+      <c r="BI60" s="99"/>
+      <c r="BJ60" s="99"/>
       <c r="BK60" s="8"/>
       <c r="BL60" s="8"/>
       <c r="BM60" s="8"/>
@@ -12504,17 +12520,17 @@
       <c r="CN60" s="46"/>
     </row>
     <row r="61" spans="3:92" ht="30" x14ac:dyDescent="0.25">
-      <c r="C61" s="84">
+      <c r="C61" s="79">
         <v>2.6</v>
       </c>
-      <c r="D61" s="89" t="s">
+      <c r="D61" s="84" t="s">
         <v>122</v>
       </c>
-      <c r="E61" s="86">
+      <c r="E61" s="81">
         <v>0</v>
       </c>
-      <c r="F61" s="87"/>
-      <c r="G61" s="87"/>
+      <c r="F61" s="82"/>
+      <c r="G61" s="82"/>
       <c r="H61" s="33"/>
       <c r="I61" s="27"/>
       <c r="J61" s="27"/>
@@ -12565,11 +12581,11 @@
       <c r="BC61" s="8"/>
       <c r="BD61" s="8"/>
       <c r="BE61" s="8"/>
-      <c r="BF61" s="107"/>
-      <c r="BG61" s="107"/>
-      <c r="BH61" s="107"/>
-      <c r="BI61" s="107"/>
-      <c r="BJ61" s="107"/>
+      <c r="BF61" s="99"/>
+      <c r="BG61" s="99"/>
+      <c r="BH61" s="99"/>
+      <c r="BI61" s="99"/>
+      <c r="BJ61" s="99"/>
       <c r="BK61" s="8"/>
       <c r="BL61" s="8"/>
       <c r="BM61" s="8"/>
@@ -12602,15 +12618,15 @@
       <c r="CN61" s="46"/>
     </row>
     <row r="62" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C62" s="97">
+      <c r="C62" s="91">
         <v>3</v>
       </c>
-      <c r="D62" s="101" t="s">
+      <c r="D62" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="101"/>
-      <c r="F62" s="101"/>
-      <c r="G62" s="101"/>
+      <c r="E62" s="108"/>
+      <c r="F62" s="108"/>
+      <c r="G62" s="108"/>
       <c r="H62" s="33"/>
       <c r="I62" s="27"/>
       <c r="J62" s="27"/>
@@ -12698,17 +12714,17 @@
       <c r="CN62" s="46"/>
     </row>
     <row r="63" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C63" s="84">
+      <c r="C63" s="79">
         <v>3.1</v>
       </c>
-      <c r="D63" s="95" t="s">
+      <c r="D63" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="E63" s="86">
+      <c r="E63" s="81">
         <v>0</v>
       </c>
-      <c r="F63" s="87"/>
-      <c r="G63" s="87"/>
+      <c r="F63" s="82"/>
+      <c r="G63" s="82"/>
       <c r="H63" s="33"/>
       <c r="I63" s="27"/>
       <c r="J63" s="27"/>
@@ -12761,9 +12777,9 @@
       <c r="BE63" s="8"/>
       <c r="BF63" s="8"/>
       <c r="BG63" s="8"/>
-      <c r="BH63" s="107"/>
-      <c r="BI63" s="107"/>
-      <c r="BJ63" s="107"/>
+      <c r="BH63" s="99"/>
+      <c r="BI63" s="99"/>
+      <c r="BJ63" s="99"/>
       <c r="BK63" s="8"/>
       <c r="BL63" s="8"/>
       <c r="BM63" s="8"/>
@@ -12796,13 +12812,13 @@
       <c r="CN63" s="46"/>
     </row>
     <row r="64" spans="3:92" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="C64" s="103"/>
-      <c r="D64" s="96" t="s">
+      <c r="C64" s="96"/>
+      <c r="D64" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="E64" s="96"/>
-      <c r="F64" s="96"/>
-      <c r="G64" s="96"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="107"/>
+      <c r="G64" s="107"/>
       <c r="H64" s="30"/>
       <c r="I64" s="8"/>
       <c r="J64" s="8"/>
@@ -12890,15 +12906,15 @@
       <c r="CN64" s="46"/>
     </row>
     <row r="65" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C65" s="97">
+      <c r="C65" s="91">
         <v>1</v>
       </c>
-      <c r="D65" s="98" t="s">
+      <c r="D65" s="92" t="s">
         <v>125</v>
       </c>
-      <c r="E65" s="98"/>
-      <c r="F65" s="99"/>
-      <c r="G65" s="99"/>
+      <c r="E65" s="92"/>
+      <c r="F65" s="93"/>
+      <c r="G65" s="93"/>
       <c r="H65" s="30"/>
       <c r="I65" s="8"/>
       <c r="J65" s="8"/>
@@ -12986,17 +13002,17 @@
       <c r="CN65" s="46"/>
     </row>
     <row r="66" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C66" s="91">
+      <c r="C66" s="86">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D66" s="95" t="s">
+      <c r="D66" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="E66" s="86">
+      <c r="E66" s="81">
         <v>0</v>
       </c>
-      <c r="F66" s="87"/>
-      <c r="G66" s="87"/>
+      <c r="F66" s="82"/>
+      <c r="G66" s="82"/>
       <c r="H66" s="33"/>
       <c r="I66" s="27"/>
       <c r="J66" s="27"/>
@@ -13054,11 +13070,11 @@
       <c r="BJ66" s="8"/>
       <c r="BK66" s="8"/>
       <c r="BL66" s="8"/>
-      <c r="BM66" s="107"/>
-      <c r="BN66" s="107"/>
-      <c r="BO66" s="107"/>
-      <c r="BP66" s="107"/>
-      <c r="BQ66" s="107"/>
+      <c r="BM66" s="99"/>
+      <c r="BN66" s="99"/>
+      <c r="BO66" s="99"/>
+      <c r="BP66" s="99"/>
+      <c r="BQ66" s="99"/>
       <c r="BR66" s="8"/>
       <c r="BS66" s="8"/>
       <c r="BT66" s="8"/>
@@ -13084,17 +13100,17 @@
       <c r="CN66" s="46"/>
     </row>
     <row r="67" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C67" s="91" t="s">
+      <c r="C67" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="D67" s="95" t="s">
+      <c r="D67" s="90" t="s">
         <v>129</v>
       </c>
-      <c r="E67" s="86">
+      <c r="E67" s="81">
         <v>0</v>
       </c>
-      <c r="F67" s="87"/>
-      <c r="G67" s="87"/>
+      <c r="F67" s="82"/>
+      <c r="G67" s="82"/>
       <c r="H67" s="33"/>
       <c r="I67" s="27"/>
       <c r="J67" s="27"/>
@@ -13152,11 +13168,11 @@
       <c r="BJ67" s="8"/>
       <c r="BK67" s="8"/>
       <c r="BL67" s="8"/>
-      <c r="BM67" s="107"/>
-      <c r="BN67" s="107"/>
-      <c r="BO67" s="107"/>
-      <c r="BP67" s="107"/>
-      <c r="BQ67" s="107"/>
+      <c r="BM67" s="99"/>
+      <c r="BN67" s="99"/>
+      <c r="BO67" s="99"/>
+      <c r="BP67" s="99"/>
+      <c r="BQ67" s="99"/>
       <c r="BR67" s="8"/>
       <c r="BS67" s="8"/>
       <c r="BT67" s="8"/>
@@ -13182,17 +13198,17 @@
       <c r="CN67" s="46"/>
     </row>
     <row r="68" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C68" s="91">
+      <c r="C68" s="86">
         <v>1.2</v>
       </c>
-      <c r="D68" s="95" t="s">
+      <c r="D68" s="90" t="s">
         <v>124</v>
       </c>
-      <c r="E68" s="86">
+      <c r="E68" s="81">
         <v>0</v>
       </c>
-      <c r="F68" s="87"/>
-      <c r="G68" s="87"/>
+      <c r="F68" s="82"/>
+      <c r="G68" s="82"/>
       <c r="H68" s="33"/>
       <c r="I68" s="27"/>
       <c r="J68" s="27"/>
@@ -13250,11 +13266,11 @@
       <c r="BJ68" s="8"/>
       <c r="BK68" s="8"/>
       <c r="BL68" s="8"/>
-      <c r="BM68" s="107"/>
-      <c r="BN68" s="107"/>
-      <c r="BO68" s="107"/>
-      <c r="BP68" s="107"/>
-      <c r="BQ68" s="107"/>
+      <c r="BM68" s="99"/>
+      <c r="BN68" s="99"/>
+      <c r="BO68" s="99"/>
+      <c r="BP68" s="99"/>
+      <c r="BQ68" s="99"/>
       <c r="BR68" s="8"/>
       <c r="BS68" s="8"/>
       <c r="BT68" s="8"/>
@@ -13280,17 +13296,17 @@
       <c r="CN68" s="46"/>
     </row>
     <row r="69" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C69" s="91" t="s">
+      <c r="C69" s="86" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="95" t="s">
+      <c r="D69" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="E69" s="86">
+      <c r="E69" s="81">
         <v>0</v>
       </c>
-      <c r="F69" s="87"/>
-      <c r="G69" s="87"/>
+      <c r="F69" s="82"/>
+      <c r="G69" s="82"/>
       <c r="H69" s="33"/>
       <c r="I69" s="27"/>
       <c r="J69" s="27"/>
@@ -13348,11 +13364,11 @@
       <c r="BJ69" s="8"/>
       <c r="BK69" s="8"/>
       <c r="BL69" s="8"/>
-      <c r="BM69" s="107"/>
-      <c r="BN69" s="107"/>
-      <c r="BO69" s="107"/>
-      <c r="BP69" s="107"/>
-      <c r="BQ69" s="107"/>
+      <c r="BM69" s="99"/>
+      <c r="BN69" s="99"/>
+      <c r="BO69" s="99"/>
+      <c r="BP69" s="99"/>
+      <c r="BQ69" s="99"/>
       <c r="BR69" s="8"/>
       <c r="BS69" s="8"/>
       <c r="BT69" s="8"/>
@@ -13378,17 +13394,17 @@
       <c r="CN69" s="46"/>
     </row>
     <row r="70" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C70" s="84">
+      <c r="C70" s="79">
         <v>1.3</v>
       </c>
-      <c r="D70" s="95" t="s">
+      <c r="D70" s="90" t="s">
         <v>126</v>
       </c>
-      <c r="E70" s="86">
+      <c r="E70" s="81">
         <v>0</v>
       </c>
-      <c r="F70" s="87"/>
-      <c r="G70" s="87"/>
+      <c r="F70" s="82"/>
+      <c r="G70" s="82"/>
       <c r="H70" s="33"/>
       <c r="I70" s="27"/>
       <c r="J70" s="27"/>
@@ -13448,14 +13464,14 @@
       <c r="BL70" s="8"/>
       <c r="BM70" s="8"/>
       <c r="BN70" s="8"/>
-      <c r="BO70" s="107"/>
-      <c r="BP70" s="107"/>
-      <c r="BQ70" s="107"/>
+      <c r="BO70" s="99"/>
+      <c r="BP70" s="99"/>
+      <c r="BQ70" s="99"/>
       <c r="BR70" s="8"/>
       <c r="BS70" s="8"/>
-      <c r="BT70" s="107"/>
-      <c r="BU70" s="107"/>
-      <c r="BV70" s="107"/>
+      <c r="BT70" s="99"/>
+      <c r="BU70" s="99"/>
+      <c r="BV70" s="99"/>
       <c r="BW70" s="8"/>
       <c r="BX70" s="8"/>
       <c r="BY70" s="8"/>
@@ -13476,17 +13492,17 @@
       <c r="CN70" s="46"/>
     </row>
     <row r="71" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C71" s="84" t="s">
+      <c r="C71" s="79" t="s">
         <v>150</v>
       </c>
-      <c r="D71" s="95" t="s">
+      <c r="D71" s="90" t="s">
         <v>127</v>
       </c>
-      <c r="E71" s="86">
+      <c r="E71" s="81">
         <v>0</v>
       </c>
-      <c r="F71" s="87"/>
-      <c r="G71" s="87"/>
+      <c r="F71" s="82"/>
+      <c r="G71" s="82"/>
       <c r="H71" s="33"/>
       <c r="I71" s="27"/>
       <c r="J71" s="27"/>
@@ -13546,14 +13562,14 @@
       <c r="BL71" s="8"/>
       <c r="BM71" s="8"/>
       <c r="BN71" s="8"/>
-      <c r="BO71" s="107"/>
-      <c r="BP71" s="107"/>
-      <c r="BQ71" s="107"/>
+      <c r="BO71" s="99"/>
+      <c r="BP71" s="99"/>
+      <c r="BQ71" s="99"/>
       <c r="BR71" s="8"/>
       <c r="BS71" s="8"/>
-      <c r="BT71" s="107"/>
-      <c r="BU71" s="107"/>
-      <c r="BV71" s="107"/>
+      <c r="BT71" s="99"/>
+      <c r="BU71" s="99"/>
+      <c r="BV71" s="99"/>
       <c r="BW71" s="8"/>
       <c r="BX71" s="8"/>
       <c r="BY71" s="8"/>
@@ -13574,17 +13590,17 @@
       <c r="CN71" s="46"/>
     </row>
     <row r="72" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C72" s="84" t="s">
+      <c r="C72" s="79" t="s">
         <v>151</v>
       </c>
-      <c r="D72" s="95" t="s">
+      <c r="D72" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="E72" s="86">
+      <c r="E72" s="81">
         <v>0</v>
       </c>
-      <c r="F72" s="87"/>
-      <c r="G72" s="87"/>
+      <c r="F72" s="82"/>
+      <c r="G72" s="82"/>
       <c r="H72" s="33"/>
       <c r="I72" s="27"/>
       <c r="J72" s="27"/>
@@ -13644,14 +13660,14 @@
       <c r="BL72" s="8"/>
       <c r="BM72" s="8"/>
       <c r="BN72" s="8"/>
-      <c r="BO72" s="107"/>
-      <c r="BP72" s="107"/>
-      <c r="BQ72" s="107"/>
+      <c r="BO72" s="99"/>
+      <c r="BP72" s="99"/>
+      <c r="BQ72" s="99"/>
       <c r="BR72" s="8"/>
       <c r="BS72" s="8"/>
-      <c r="BT72" s="107"/>
-      <c r="BU72" s="107"/>
-      <c r="BV72" s="107"/>
+      <c r="BT72" s="99"/>
+      <c r="BU72" s="99"/>
+      <c r="BV72" s="99"/>
       <c r="BW72" s="8"/>
       <c r="BX72" s="8"/>
       <c r="BY72" s="8"/>
@@ -13672,17 +13688,17 @@
       <c r="CN72" s="46"/>
     </row>
     <row r="73" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C73" s="84">
+      <c r="C73" s="79">
         <v>1.4</v>
       </c>
-      <c r="D73" s="95" t="s">
+      <c r="D73" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="E73" s="86">
+      <c r="E73" s="81">
         <v>0</v>
       </c>
-      <c r="F73" s="87"/>
-      <c r="G73" s="87"/>
+      <c r="F73" s="82"/>
+      <c r="G73" s="82"/>
       <c r="H73" s="33"/>
       <c r="I73" s="27"/>
       <c r="J73" s="27"/>
@@ -13742,14 +13758,14 @@
       <c r="BL73" s="8"/>
       <c r="BM73" s="8"/>
       <c r="BN73" s="8"/>
-      <c r="BO73" s="107"/>
-      <c r="BP73" s="107"/>
-      <c r="BQ73" s="107"/>
+      <c r="BO73" s="99"/>
+      <c r="BP73" s="99"/>
+      <c r="BQ73" s="99"/>
       <c r="BR73" s="8"/>
       <c r="BS73" s="8"/>
-      <c r="BT73" s="107"/>
-      <c r="BU73" s="107"/>
-      <c r="BV73" s="107"/>
+      <c r="BT73" s="99"/>
+      <c r="BU73" s="99"/>
+      <c r="BV73" s="99"/>
       <c r="BW73" s="8"/>
       <c r="BX73" s="8"/>
       <c r="BY73" s="8"/>
@@ -13770,17 +13786,17 @@
       <c r="CN73" s="46"/>
     </row>
     <row r="74" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C74" s="84">
+      <c r="C74" s="79">
         <v>1.5</v>
       </c>
-      <c r="D74" s="95" t="s">
+      <c r="D74" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="E74" s="86">
+      <c r="E74" s="81">
         <v>0</v>
       </c>
-      <c r="F74" s="87"/>
-      <c r="G74" s="87"/>
+      <c r="F74" s="82"/>
+      <c r="G74" s="82"/>
       <c r="H74" s="33"/>
       <c r="I74" s="27"/>
       <c r="J74" s="27"/>
@@ -13846,9 +13862,9 @@
       <c r="BR74" s="8"/>
       <c r="BS74" s="8"/>
       <c r="BT74" s="8"/>
-      <c r="BU74" s="107"/>
-      <c r="BV74" s="107"/>
-      <c r="BW74" s="107"/>
+      <c r="BU74" s="99"/>
+      <c r="BV74" s="99"/>
+      <c r="BW74" s="99"/>
       <c r="BX74" s="47"/>
       <c r="BY74" s="8"/>
       <c r="BZ74" s="8"/>
@@ -13868,17 +13884,17 @@
       <c r="CN74" s="46"/>
     </row>
     <row r="75" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C75" s="84" t="s">
+      <c r="C75" s="79" t="s">
         <v>152</v>
       </c>
-      <c r="D75" s="95" t="s">
+      <c r="D75" s="90" t="s">
         <v>132</v>
       </c>
-      <c r="E75" s="86">
+      <c r="E75" s="81">
         <v>0</v>
       </c>
-      <c r="F75" s="87"/>
-      <c r="G75" s="87"/>
+      <c r="F75" s="82"/>
+      <c r="G75" s="82"/>
       <c r="H75" s="33"/>
       <c r="I75" s="27"/>
       <c r="J75" s="27"/>
@@ -13944,9 +13960,9 @@
       <c r="BR75" s="8"/>
       <c r="BS75" s="8"/>
       <c r="BT75" s="8"/>
-      <c r="BU75" s="107"/>
-      <c r="BV75" s="107"/>
-      <c r="BW75" s="107"/>
+      <c r="BU75" s="99"/>
+      <c r="BV75" s="99"/>
+      <c r="BW75" s="99"/>
       <c r="BX75" s="47"/>
       <c r="BY75" s="8"/>
       <c r="BZ75" s="8"/>
@@ -13966,17 +13982,17 @@
       <c r="CN75" s="46"/>
     </row>
     <row r="76" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C76" s="84">
+      <c r="C76" s="79">
         <v>1.6</v>
       </c>
-      <c r="D76" s="95" t="s">
+      <c r="D76" s="90" t="s">
         <v>133</v>
       </c>
-      <c r="E76" s="86">
+      <c r="E76" s="81">
         <v>0</v>
       </c>
-      <c r="F76" s="87"/>
-      <c r="G76" s="87"/>
+      <c r="F76" s="82"/>
+      <c r="G76" s="82"/>
       <c r="H76" s="33"/>
       <c r="I76" s="27"/>
       <c r="J76" s="27"/>
@@ -14042,9 +14058,9 @@
       <c r="BR76" s="8"/>
       <c r="BS76" s="8"/>
       <c r="BT76" s="8"/>
-      <c r="BU76" s="107"/>
-      <c r="BV76" s="107"/>
-      <c r="BW76" s="107"/>
+      <c r="BU76" s="99"/>
+      <c r="BV76" s="99"/>
+      <c r="BW76" s="99"/>
       <c r="BX76" s="47"/>
       <c r="BY76" s="8"/>
       <c r="BZ76" s="8"/>
@@ -14064,17 +14080,17 @@
       <c r="CN76" s="46"/>
     </row>
     <row r="77" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C77" s="84" t="s">
+      <c r="C77" s="79" t="s">
         <v>153</v>
       </c>
-      <c r="D77" s="95" t="s">
+      <c r="D77" s="90" t="s">
         <v>134</v>
       </c>
-      <c r="E77" s="86">
+      <c r="E77" s="81">
         <v>0</v>
       </c>
-      <c r="F77" s="87"/>
-      <c r="G77" s="87"/>
+      <c r="F77" s="82"/>
+      <c r="G77" s="82"/>
       <c r="H77" s="33"/>
       <c r="I77" s="27"/>
       <c r="J77" s="27"/>
@@ -14140,9 +14156,9 @@
       <c r="BR77" s="8"/>
       <c r="BS77" s="8"/>
       <c r="BT77" s="8"/>
-      <c r="BU77" s="107"/>
-      <c r="BV77" s="107"/>
-      <c r="BW77" s="107"/>
+      <c r="BU77" s="99"/>
+      <c r="BV77" s="99"/>
+      <c r="BW77" s="99"/>
       <c r="BX77" s="47"/>
       <c r="BY77" s="47"/>
       <c r="BZ77" s="8"/>
@@ -14162,15 +14178,15 @@
       <c r="CN77" s="46"/>
     </row>
     <row r="78" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C78" s="97">
+      <c r="C78" s="91">
         <v>2</v>
       </c>
-      <c r="D78" s="101" t="s">
+      <c r="D78" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E78" s="101"/>
-      <c r="F78" s="101"/>
-      <c r="G78" s="101"/>
+      <c r="E78" s="108"/>
+      <c r="F78" s="108"/>
+      <c r="G78" s="108"/>
       <c r="H78" s="33"/>
       <c r="I78" s="27"/>
       <c r="J78" s="27"/>
@@ -14258,17 +14274,17 @@
       <c r="CN78" s="46"/>
     </row>
     <row r="79" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C79" s="92">
+      <c r="C79" s="87">
         <v>2.1</v>
       </c>
-      <c r="D79" s="95" t="s">
+      <c r="D79" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="E79" s="86">
+      <c r="E79" s="81">
         <v>0</v>
       </c>
-      <c r="F79" s="87"/>
-      <c r="G79" s="87"/>
+      <c r="F79" s="82"/>
+      <c r="G79" s="82"/>
       <c r="H79" s="33"/>
       <c r="I79" s="27"/>
       <c r="J79" s="27"/>
@@ -14334,10 +14350,10 @@
       <c r="BR79" s="8"/>
       <c r="BS79" s="8"/>
       <c r="BT79" s="8"/>
-      <c r="BU79" s="107"/>
-      <c r="BV79" s="107"/>
-      <c r="BW79" s="107"/>
-      <c r="BX79" s="107"/>
+      <c r="BU79" s="99"/>
+      <c r="BV79" s="99"/>
+      <c r="BW79" s="99"/>
+      <c r="BX79" s="99"/>
       <c r="BY79" s="8"/>
       <c r="BZ79" s="8"/>
       <c r="CA79" s="8"/>
@@ -14356,17 +14372,17 @@
       <c r="CN79" s="46"/>
     </row>
     <row r="80" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C80" s="84">
+      <c r="C80" s="79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D80" s="95" t="s">
+      <c r="D80" s="90" t="s">
         <v>136</v>
       </c>
-      <c r="E80" s="86">
+      <c r="E80" s="81">
         <v>0</v>
       </c>
-      <c r="F80" s="87"/>
-      <c r="G80" s="87"/>
+      <c r="F80" s="82"/>
+      <c r="G80" s="82"/>
       <c r="H80" s="33"/>
       <c r="I80" s="27"/>
       <c r="J80" s="27"/>
@@ -14432,10 +14448,10 @@
       <c r="BR80" s="8"/>
       <c r="BS80" s="8"/>
       <c r="BT80" s="8"/>
-      <c r="BU80" s="107"/>
-      <c r="BV80" s="107"/>
-      <c r="BW80" s="107"/>
-      <c r="BX80" s="107"/>
+      <c r="BU80" s="99"/>
+      <c r="BV80" s="99"/>
+      <c r="BW80" s="99"/>
+      <c r="BX80" s="99"/>
       <c r="BY80" s="8"/>
       <c r="BZ80" s="8"/>
       <c r="CA80" s="8"/>
@@ -14454,17 +14470,17 @@
       <c r="CN80" s="46"/>
     </row>
     <row r="81" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C81" s="84">
+      <c r="C81" s="79">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D81" s="95" t="s">
+      <c r="D81" s="90" t="s">
         <v>154</v>
       </c>
-      <c r="E81" s="86">
+      <c r="E81" s="81">
         <v>0</v>
       </c>
-      <c r="F81" s="87"/>
-      <c r="G81" s="87"/>
+      <c r="F81" s="82"/>
+      <c r="G81" s="82"/>
       <c r="H81" s="33"/>
       <c r="I81" s="27"/>
       <c r="J81" s="27"/>
@@ -14530,10 +14546,10 @@
       <c r="BR81" s="8"/>
       <c r="BS81" s="8"/>
       <c r="BT81" s="8"/>
-      <c r="BU81" s="107"/>
-      <c r="BV81" s="107"/>
-      <c r="BW81" s="107"/>
-      <c r="BX81" s="107"/>
+      <c r="BU81" s="99"/>
+      <c r="BV81" s="99"/>
+      <c r="BW81" s="99"/>
+      <c r="BX81" s="99"/>
       <c r="BY81" s="8"/>
       <c r="BZ81" s="8"/>
       <c r="CA81" s="8"/>
@@ -14552,13 +14568,13 @@
       <c r="CN81" s="46"/>
     </row>
     <row r="82" spans="3:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C82" s="103"/>
-      <c r="D82" s="96" t="s">
+      <c r="C82" s="96"/>
+      <c r="D82" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="E82" s="96"/>
-      <c r="F82" s="96"/>
-      <c r="G82" s="104"/>
+      <c r="E82" s="107"/>
+      <c r="F82" s="107"/>
+      <c r="G82" s="109"/>
       <c r="H82" s="30"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
@@ -14646,15 +14662,15 @@
       <c r="CN82" s="46"/>
     </row>
     <row r="83" spans="3:92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C83" s="97">
+      <c r="C83" s="91">
         <v>1</v>
       </c>
-      <c r="D83" s="98" t="s">
+      <c r="D83" s="92" t="s">
         <v>125</v>
       </c>
-      <c r="E83" s="98"/>
-      <c r="F83" s="99"/>
-      <c r="G83" s="99"/>
+      <c r="E83" s="92"/>
+      <c r="F83" s="93"/>
+      <c r="G83" s="93"/>
       <c r="H83" s="30"/>
       <c r="I83" s="8"/>
       <c r="J83" s="8"/>
@@ -14742,17 +14758,17 @@
       <c r="CN83" s="46"/>
     </row>
     <row r="84" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C84" s="84">
+      <c r="C84" s="79">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D84" s="89" t="s">
+      <c r="D84" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="E84" s="86">
+      <c r="E84" s="81">
         <v>0</v>
       </c>
-      <c r="F84" s="87"/>
-      <c r="G84" s="87"/>
+      <c r="F84" s="82"/>
+      <c r="G84" s="82"/>
       <c r="H84" s="33"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
@@ -14824,11 +14840,11 @@
       <c r="BX84" s="8"/>
       <c r="BY84" s="8"/>
       <c r="BZ84" s="8"/>
-      <c r="CA84" s="107"/>
-      <c r="CB84" s="107"/>
-      <c r="CC84" s="107"/>
-      <c r="CD84" s="107"/>
-      <c r="CE84" s="107"/>
+      <c r="CA84" s="99"/>
+      <c r="CB84" s="99"/>
+      <c r="CC84" s="99"/>
+      <c r="CD84" s="99"/>
+      <c r="CE84" s="99"/>
       <c r="CF84" s="8"/>
       <c r="CG84" s="8"/>
       <c r="CH84" s="8"/>
@@ -14840,17 +14856,17 @@
       <c r="CN84" s="46"/>
     </row>
     <row r="85" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C85" s="91">
+      <c r="C85" s="86">
         <v>1.2</v>
       </c>
-      <c r="D85" s="89" t="s">
+      <c r="D85" s="84" t="s">
         <v>135</v>
       </c>
-      <c r="E85" s="86">
+      <c r="E85" s="81">
         <v>0</v>
       </c>
-      <c r="F85" s="87"/>
-      <c r="G85" s="87"/>
+      <c r="F85" s="82"/>
+      <c r="G85" s="82"/>
       <c r="H85" s="33"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -14922,11 +14938,11 @@
       <c r="BX85" s="8"/>
       <c r="BY85" s="8"/>
       <c r="BZ85" s="8"/>
-      <c r="CA85" s="107"/>
-      <c r="CB85" s="107"/>
-      <c r="CC85" s="107"/>
-      <c r="CD85" s="107"/>
-      <c r="CE85" s="107"/>
+      <c r="CA85" s="99"/>
+      <c r="CB85" s="99"/>
+      <c r="CC85" s="99"/>
+      <c r="CD85" s="99"/>
+      <c r="CE85" s="99"/>
       <c r="CF85" s="8"/>
       <c r="CG85" s="8"/>
       <c r="CH85" s="8"/>
@@ -14938,15 +14954,15 @@
       <c r="CN85" s="46"/>
     </row>
     <row r="86" spans="3:92" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C86" s="97">
+      <c r="C86" s="91">
         <v>2</v>
       </c>
-      <c r="D86" s="101" t="s">
+      <c r="D86" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E86" s="101"/>
-      <c r="F86" s="101"/>
-      <c r="G86" s="101"/>
+      <c r="E86" s="108"/>
+      <c r="F86" s="108"/>
+      <c r="G86" s="108"/>
       <c r="H86" s="33"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
@@ -15034,17 +15050,17 @@
       <c r="CN86" s="46"/>
     </row>
     <row r="87" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C87" s="84">
+      <c r="C87" s="79">
         <v>2.1</v>
       </c>
-      <c r="D87" s="89" t="s">
+      <c r="D87" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="E87" s="86">
+      <c r="E87" s="81">
         <v>0</v>
       </c>
-      <c r="F87" s="87"/>
-      <c r="G87" s="87"/>
+      <c r="F87" s="82"/>
+      <c r="G87" s="82"/>
       <c r="H87" s="33"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -15117,10 +15133,10 @@
       <c r="BY87" s="8"/>
       <c r="BZ87" s="8"/>
       <c r="CA87" s="8"/>
-      <c r="CB87" s="107"/>
-      <c r="CC87" s="107"/>
-      <c r="CD87" s="107"/>
-      <c r="CE87" s="107"/>
+      <c r="CB87" s="99"/>
+      <c r="CC87" s="99"/>
+      <c r="CD87" s="99"/>
+      <c r="CE87" s="99"/>
       <c r="CF87" s="8"/>
       <c r="CG87" s="8"/>
       <c r="CH87" s="8"/>
@@ -15132,17 +15148,17 @@
       <c r="CN87" s="46"/>
     </row>
     <row r="88" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C88" s="91">
+      <c r="C88" s="86">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D88" s="89" t="s">
+      <c r="D88" s="84" t="s">
         <v>137</v>
       </c>
-      <c r="E88" s="86">
+      <c r="E88" s="81">
         <v>0</v>
       </c>
-      <c r="F88" s="87"/>
-      <c r="G88" s="87"/>
+      <c r="F88" s="82"/>
+      <c r="G88" s="82"/>
       <c r="H88" s="33"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
@@ -15215,10 +15231,10 @@
       <c r="BY88" s="8"/>
       <c r="BZ88" s="8"/>
       <c r="CA88" s="8"/>
-      <c r="CB88" s="107"/>
-      <c r="CC88" s="107"/>
-      <c r="CD88" s="107"/>
-      <c r="CE88" s="107"/>
+      <c r="CB88" s="99"/>
+      <c r="CC88" s="99"/>
+      <c r="CD88" s="99"/>
+      <c r="CE88" s="99"/>
       <c r="CF88" s="8"/>
       <c r="CG88" s="8"/>
       <c r="CH88" s="8"/>
@@ -15230,17 +15246,17 @@
       <c r="CN88" s="46"/>
     </row>
     <row r="89" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C89" s="84">
+      <c r="C89" s="79">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D89" s="89" t="s">
+      <c r="D89" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="E89" s="86">
+      <c r="E89" s="81">
         <v>0</v>
       </c>
-      <c r="F89" s="87"/>
-      <c r="G89" s="87"/>
+      <c r="F89" s="82"/>
+      <c r="G89" s="82"/>
       <c r="H89" s="33"/>
       <c r="I89" s="8"/>
       <c r="J89" s="8"/>
@@ -15313,10 +15329,10 @@
       <c r="BY89" s="8"/>
       <c r="BZ89" s="8"/>
       <c r="CA89" s="8"/>
-      <c r="CB89" s="107"/>
-      <c r="CC89" s="107"/>
-      <c r="CD89" s="107"/>
-      <c r="CE89" s="107"/>
+      <c r="CB89" s="99"/>
+      <c r="CC89" s="99"/>
+      <c r="CD89" s="99"/>
+      <c r="CE89" s="99"/>
       <c r="CF89" s="8"/>
       <c r="CG89" s="8"/>
       <c r="CH89" s="8"/>
@@ -15328,17 +15344,17 @@
       <c r="CN89" s="46"/>
     </row>
     <row r="90" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C90" s="91">
+      <c r="C90" s="86">
         <v>2.4</v>
       </c>
-      <c r="D90" s="89" t="s">
+      <c r="D90" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="E90" s="86">
+      <c r="E90" s="81">
         <v>0</v>
       </c>
-      <c r="F90" s="87"/>
-      <c r="G90" s="87"/>
+      <c r="F90" s="82"/>
+      <c r="G90" s="82"/>
       <c r="H90" s="33"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -15411,10 +15427,10 @@
       <c r="BY90" s="8"/>
       <c r="BZ90" s="8"/>
       <c r="CA90" s="8"/>
-      <c r="CB90" s="107"/>
-      <c r="CC90" s="107"/>
-      <c r="CD90" s="107"/>
-      <c r="CE90" s="107"/>
+      <c r="CB90" s="99"/>
+      <c r="CC90" s="99"/>
+      <c r="CD90" s="99"/>
+      <c r="CE90" s="99"/>
       <c r="CF90" s="8"/>
       <c r="CG90" s="8"/>
       <c r="CH90" s="8"/>
@@ -15426,17 +15442,17 @@
       <c r="CN90" s="46"/>
     </row>
     <row r="91" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C91" s="84">
+      <c r="C91" s="79">
         <v>2.5</v>
       </c>
-      <c r="D91" s="89" t="s">
+      <c r="D91" s="84" t="s">
         <v>64</v>
       </c>
-      <c r="E91" s="86">
+      <c r="E91" s="81">
         <v>0</v>
       </c>
-      <c r="F91" s="87"/>
-      <c r="G91" s="87"/>
+      <c r="F91" s="82"/>
+      <c r="G91" s="82"/>
       <c r="H91" s="33"/>
       <c r="I91" s="8"/>
       <c r="J91" s="8"/>
@@ -15509,10 +15525,10 @@
       <c r="BY91" s="8"/>
       <c r="BZ91" s="8"/>
       <c r="CA91" s="8"/>
-      <c r="CB91" s="107"/>
-      <c r="CC91" s="107"/>
-      <c r="CD91" s="107"/>
-      <c r="CE91" s="107"/>
+      <c r="CB91" s="99"/>
+      <c r="CC91" s="99"/>
+      <c r="CD91" s="99"/>
+      <c r="CE91" s="99"/>
       <c r="CF91" s="8"/>
       <c r="CG91" s="8"/>
       <c r="CH91" s="8"/>
@@ -15524,17 +15540,17 @@
       <c r="CN91" s="46"/>
     </row>
     <row r="92" spans="3:92" x14ac:dyDescent="0.25">
-      <c r="C92" s="91">
+      <c r="C92" s="86">
         <v>2.6</v>
       </c>
-      <c r="D92" s="89" t="s">
+      <c r="D92" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="E92" s="86">
+      <c r="E92" s="81">
         <v>0</v>
       </c>
-      <c r="F92" s="87"/>
-      <c r="G92" s="87"/>
+      <c r="F92" s="82"/>
+      <c r="G92" s="82"/>
       <c r="H92" s="35"/>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
@@ -15609,8 +15625,8 @@
       <c r="CA92" s="36"/>
       <c r="CB92" s="66"/>
       <c r="CC92" s="66"/>
-      <c r="CD92" s="108"/>
-      <c r="CE92" s="108"/>
+      <c r="CD92" s="100"/>
+      <c r="CE92" s="100"/>
       <c r="CF92" s="36"/>
       <c r="CG92" s="36"/>
       <c r="CH92" s="36"/>
@@ -15623,6 +15639,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="AD2:AJ2"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D64:G64"/>
     <mergeCell ref="BT2:BZ2"/>
     <mergeCell ref="CA2:CG2"/>
     <mergeCell ref="CH2:CN2"/>
@@ -15639,13 +15662,6 @@
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="W2:AC2"/>
-    <mergeCell ref="AD2:AJ2"/>
-    <mergeCell ref="D82:G82"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D64:G64"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E10 E13:E16 E18:E24">
     <cfRule type="dataBar" priority="20">

</xml_diff>

<commit_message>
Added more numbers to charts
</commit_message>
<xml_diff>
--- a/documentation/Charts/Charts-WIP.xlsx
+++ b/documentation/Charts/Charts-WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rex\Desktop\Project template code\Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F88D29-40FC-4D35-8A0D-98720055CBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115282E2-4E5B-4E8E-B7FB-6AA490CC7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{5FED8FEB-A2F0-45E6-B7D6-62982F9FC7E5}"/>
   </bookViews>
@@ -1436,10 +1436,10 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2702,10 +2702,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Burndown!$C$30:$E$30</c:f>
+              <c:f>Burndown!$C$30:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>350</c:v>
                 </c:pt>
@@ -2714,6 +2714,18 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>223</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4414,8 +4426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3693011-238F-42BC-B2CC-2AF5AE5811AA}">
   <dimension ref="B4:M87"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U39" sqref="U39"/>
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5129,15 +5141,29 @@
         <v>2</v>
       </c>
       <c r="E29" s="12">
-        <v>1</v>
-      </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
+        <v>2</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0</v>
+      </c>
+      <c r="G29" s="12">
+        <v>0</v>
+      </c>
+      <c r="H29" s="12">
+        <v>0</v>
+      </c>
+      <c r="I29" s="12">
+        <v>0</v>
+      </c>
+      <c r="J29" s="12">
+        <v>0</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
+        <v>0</v>
+      </c>
       <c r="M29" s="12">
         <v>3</v>
       </c>
@@ -5152,14 +5178,30 @@
       <c r="D30" s="12">
         <v>0</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
+      <c r="E30" s="12">
+        <v>2</v>
+      </c>
+      <c r="F30" s="12">
+        <v>2</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1</v>
+      </c>
+      <c r="H30" s="12">
+        <v>1</v>
+      </c>
+      <c r="I30" s="12">
+        <v>1</v>
+      </c>
+      <c r="J30" s="12">
+        <v>0</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>0</v>
+      </c>
       <c r="M30" s="12">
         <v>5</v>
       </c>
@@ -5174,14 +5216,30 @@
       <c r="D31" s="12">
         <v>0</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
+      <c r="E31" s="12">
+        <v>2</v>
+      </c>
+      <c r="F31" s="12">
+        <v>2</v>
+      </c>
+      <c r="G31" s="12">
+        <v>1</v>
+      </c>
+      <c r="H31" s="12">
+        <v>1</v>
+      </c>
+      <c r="I31" s="12">
+        <v>1</v>
+      </c>
+      <c r="J31" s="12">
+        <v>0</v>
+      </c>
+      <c r="K31" s="12">
+        <v>0</v>
+      </c>
+      <c r="L31" s="12">
+        <v>0</v>
+      </c>
       <c r="M31" s="12">
         <v>4</v>
       </c>
@@ -5196,14 +5254,30 @@
       <c r="D32" s="12">
         <v>0</v>
       </c>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
+      <c r="E32" s="12">
+        <v>2</v>
+      </c>
+      <c r="F32" s="12">
+        <v>2</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1</v>
+      </c>
+      <c r="H32" s="12">
+        <v>1</v>
+      </c>
+      <c r="I32" s="12">
+        <v>1</v>
+      </c>
+      <c r="J32" s="12">
+        <v>0</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0</v>
+      </c>
       <c r="M32" s="12">
         <v>4</v>
       </c>
@@ -5218,14 +5292,30 @@
       <c r="D33" s="12">
         <v>0</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
+      <c r="E33" s="12">
+        <v>2</v>
+      </c>
+      <c r="F33" s="12">
+        <v>2</v>
+      </c>
+      <c r="G33" s="12">
+        <v>1</v>
+      </c>
+      <c r="H33" s="12">
+        <v>1</v>
+      </c>
+      <c r="I33" s="12">
+        <v>1</v>
+      </c>
+      <c r="J33" s="12">
+        <v>0</v>
+      </c>
+      <c r="K33" s="12">
+        <v>0</v>
+      </c>
+      <c r="L33" s="12">
+        <v>0</v>
+      </c>
       <c r="M33" s="12">
         <v>5</v>
       </c>
@@ -5240,14 +5330,30 @@
       <c r="D34" s="12">
         <v>0</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
+      <c r="E34" s="12">
+        <v>2</v>
+      </c>
+      <c r="F34" s="12">
+        <v>2</v>
+      </c>
+      <c r="G34" s="12">
+        <v>1</v>
+      </c>
+      <c r="H34" s="12">
+        <v>1</v>
+      </c>
+      <c r="I34" s="12">
+        <v>1</v>
+      </c>
+      <c r="J34" s="12">
+        <v>0</v>
+      </c>
+      <c r="K34" s="12">
+        <v>0</v>
+      </c>
+      <c r="L34" s="12">
+        <v>0</v>
+      </c>
       <c r="M34" s="12">
         <v>4</v>
       </c>
@@ -5262,14 +5368,30 @@
       <c r="D35" s="12">
         <v>0</v>
       </c>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
+      <c r="E35" s="12">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <v>1</v>
+      </c>
+      <c r="I35" s="12">
+        <v>2</v>
+      </c>
+      <c r="J35" s="12">
+        <v>2</v>
+      </c>
+      <c r="K35" s="12">
+        <v>1</v>
+      </c>
+      <c r="L35" s="12">
+        <v>0</v>
+      </c>
       <c r="M35" s="12">
         <v>7</v>
       </c>
@@ -5284,14 +5406,30 @@
       <c r="D36" s="12">
         <v>0</v>
       </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
+      <c r="E36" s="12">
+        <v>0</v>
+      </c>
+      <c r="F36" s="12">
+        <v>0</v>
+      </c>
+      <c r="G36" s="12">
+        <v>0</v>
+      </c>
+      <c r="H36" s="12">
+        <v>1</v>
+      </c>
+      <c r="I36" s="12">
+        <v>2</v>
+      </c>
+      <c r="J36" s="12">
+        <v>2</v>
+      </c>
+      <c r="K36" s="12">
+        <v>1</v>
+      </c>
+      <c r="L36" s="12">
+        <v>0</v>
+      </c>
       <c r="M36" s="12">
         <v>7</v>
       </c>
@@ -5306,14 +5444,30 @@
       <c r="D37" s="12">
         <v>0</v>
       </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
+      <c r="E37" s="12">
+        <v>0</v>
+      </c>
+      <c r="F37" s="12">
+        <v>0</v>
+      </c>
+      <c r="G37" s="12">
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <v>1</v>
+      </c>
+      <c r="I37" s="12">
+        <v>2</v>
+      </c>
+      <c r="J37" s="12">
+        <v>2</v>
+      </c>
+      <c r="K37" s="12">
+        <v>1</v>
+      </c>
+      <c r="L37" s="12">
+        <v>0</v>
+      </c>
       <c r="M37" s="12">
         <v>4</v>
       </c>
@@ -5328,14 +5482,30 @@
       <c r="D38" s="12">
         <v>0</v>
       </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12"/>
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
+        <v>0</v>
+      </c>
+      <c r="H38" s="12">
+        <v>1</v>
+      </c>
+      <c r="I38" s="12">
+        <v>2</v>
+      </c>
+      <c r="J38" s="12">
+        <v>2</v>
+      </c>
+      <c r="K38" s="12">
+        <v>1</v>
+      </c>
+      <c r="L38" s="12">
+        <v>0</v>
+      </c>
       <c r="M38" s="12">
         <v>8</v>
       </c>
@@ -5350,14 +5520,30 @@
       <c r="D39" s="12">
         <v>0</v>
       </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-      <c r="L39" s="12"/>
+      <c r="E39" s="12">
+        <v>0</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
+        <v>0</v>
+      </c>
+      <c r="H39" s="12">
+        <v>0</v>
+      </c>
+      <c r="I39" s="12">
+        <v>0</v>
+      </c>
+      <c r="J39" s="12">
+        <v>2</v>
+      </c>
+      <c r="K39" s="12">
+        <v>2</v>
+      </c>
+      <c r="L39" s="12">
+        <v>2</v>
+      </c>
       <c r="M39" s="12">
         <v>8</v>
       </c>
@@ -5372,14 +5558,30 @@
       <c r="D40" s="12">
         <v>0</v>
       </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-      <c r="L40" s="12"/>
+      <c r="E40" s="12">
+        <v>0</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0</v>
+      </c>
+      <c r="G40" s="12">
+        <v>0</v>
+      </c>
+      <c r="H40" s="12">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <v>0</v>
+      </c>
+      <c r="J40" s="12">
+        <v>2</v>
+      </c>
+      <c r="K40" s="12">
+        <v>2</v>
+      </c>
+      <c r="L40" s="12">
+        <v>2</v>
+      </c>
       <c r="M40" s="12">
         <v>8</v>
       </c>
@@ -5394,14 +5596,30 @@
       <c r="D41" s="12">
         <v>0</v>
       </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-      <c r="L41" s="12"/>
+      <c r="E41" s="12">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0</v>
+      </c>
+      <c r="G41" s="12">
+        <v>0</v>
+      </c>
+      <c r="H41" s="12">
+        <v>0</v>
+      </c>
+      <c r="I41" s="12">
+        <v>0</v>
+      </c>
+      <c r="J41" s="12">
+        <v>2</v>
+      </c>
+      <c r="K41" s="12">
+        <v>2</v>
+      </c>
+      <c r="L41" s="12">
+        <v>2</v>
+      </c>
       <c r="M41" s="12">
         <v>6</v>
       </c>
@@ -5431,7 +5649,7 @@
       </c>
       <c r="C43" s="70">
         <f>SUM(C29:L41)</f>
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="D43" s="74"/>
       <c r="E43" s="74"/>
@@ -5450,7 +5668,7 @@
       </c>
       <c r="C44" s="70">
         <f>SUM(C42,-(C43))</f>
-        <v>68</v>
+        <v>-10</v>
       </c>
       <c r="D44" s="76"/>
       <c r="E44" s="77"/>
@@ -5525,16 +5743,36 @@
       <c r="B48" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-      <c r="L48" s="12"/>
+      <c r="C48" s="12">
+        <v>3</v>
+      </c>
+      <c r="D48" s="12">
+        <v>3</v>
+      </c>
+      <c r="E48" s="12">
+        <v>2</v>
+      </c>
+      <c r="F48" s="12">
+        <v>1</v>
+      </c>
+      <c r="G48" s="12">
+        <v>1</v>
+      </c>
+      <c r="H48" s="12">
+        <v>0</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0</v>
+      </c>
+      <c r="J48" s="12">
+        <v>0</v>
+      </c>
+      <c r="K48" s="12">
+        <v>0</v>
+      </c>
+      <c r="L48" s="12">
+        <v>0</v>
+      </c>
       <c r="M48" s="12">
         <v>10</v>
       </c>
@@ -5543,16 +5781,36 @@
       <c r="B49" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-      <c r="L49" s="12"/>
+      <c r="C49" s="12">
+        <v>1</v>
+      </c>
+      <c r="D49" s="12">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12">
+        <v>2</v>
+      </c>
+      <c r="F49" s="12">
+        <v>2</v>
+      </c>
+      <c r="G49" s="12">
+        <v>3</v>
+      </c>
+      <c r="H49" s="12">
+        <v>0</v>
+      </c>
+      <c r="I49" s="12">
+        <v>0</v>
+      </c>
+      <c r="J49" s="12">
+        <v>0</v>
+      </c>
+      <c r="K49" s="12">
+        <v>0</v>
+      </c>
+      <c r="L49" s="12">
+        <v>0</v>
+      </c>
       <c r="M49" s="12">
         <v>8</v>
       </c>
@@ -5561,16 +5819,36 @@
       <c r="B50" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12"/>
+      <c r="C50" s="12">
+        <v>1</v>
+      </c>
+      <c r="D50" s="12">
+        <v>1</v>
+      </c>
+      <c r="E50" s="12">
+        <v>2</v>
+      </c>
+      <c r="F50" s="12">
+        <v>2</v>
+      </c>
+      <c r="G50" s="12">
+        <v>3</v>
+      </c>
+      <c r="H50" s="12">
+        <v>0</v>
+      </c>
+      <c r="I50" s="12">
+        <v>0</v>
+      </c>
+      <c r="J50" s="12">
+        <v>0</v>
+      </c>
+      <c r="K50" s="12">
+        <v>0</v>
+      </c>
+      <c r="L50" s="12">
+        <v>0</v>
+      </c>
       <c r="M50" s="12">
         <v>8</v>
       </c>
@@ -5579,16 +5857,36 @@
       <c r="B51" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
+      <c r="C51" s="12">
+        <v>0</v>
+      </c>
+      <c r="D51" s="12">
+        <v>0</v>
+      </c>
+      <c r="E51" s="12">
+        <v>1</v>
+      </c>
+      <c r="F51" s="12">
+        <v>2</v>
+      </c>
+      <c r="G51" s="12">
+        <v>2</v>
+      </c>
+      <c r="H51" s="12">
+        <v>2</v>
+      </c>
+      <c r="I51" s="12">
+        <v>1</v>
+      </c>
+      <c r="J51" s="12">
+        <v>0</v>
+      </c>
+      <c r="K51" s="12">
+        <v>0</v>
+      </c>
+      <c r="L51" s="12">
+        <v>0</v>
+      </c>
       <c r="M51" s="12">
         <v>8</v>
       </c>
@@ -5597,16 +5895,36 @@
       <c r="B52" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-      <c r="L52" s="12"/>
+      <c r="C52" s="12">
+        <v>0</v>
+      </c>
+      <c r="D52" s="12">
+        <v>0</v>
+      </c>
+      <c r="E52" s="12">
+        <v>1</v>
+      </c>
+      <c r="F52" s="12">
+        <v>2</v>
+      </c>
+      <c r="G52" s="12">
+        <v>2</v>
+      </c>
+      <c r="H52" s="12">
+        <v>2</v>
+      </c>
+      <c r="I52" s="12">
+        <v>1</v>
+      </c>
+      <c r="J52" s="12">
+        <v>0</v>
+      </c>
+      <c r="K52" s="12">
+        <v>0</v>
+      </c>
+      <c r="L52" s="12">
+        <v>0</v>
+      </c>
       <c r="M52" s="12">
         <v>6</v>
       </c>
@@ -5615,16 +5933,36 @@
       <c r="B53" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
+      <c r="C53" s="12">
+        <v>0</v>
+      </c>
+      <c r="D53" s="12">
+        <v>0</v>
+      </c>
+      <c r="E53" s="12">
+        <v>1</v>
+      </c>
+      <c r="F53" s="12">
+        <v>2</v>
+      </c>
+      <c r="G53" s="12">
+        <v>2</v>
+      </c>
+      <c r="H53" s="12">
+        <v>2</v>
+      </c>
+      <c r="I53" s="12">
+        <v>1</v>
+      </c>
+      <c r="J53" s="12">
+        <v>0</v>
+      </c>
+      <c r="K53" s="12">
+        <v>0</v>
+      </c>
+      <c r="L53" s="12">
+        <v>0</v>
+      </c>
       <c r="M53" s="12">
         <v>6</v>
       </c>
@@ -5633,16 +5971,36 @@
       <c r="B54" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
+      <c r="C54" s="12">
+        <v>0</v>
+      </c>
+      <c r="D54" s="12">
+        <v>0</v>
+      </c>
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
+        <v>0</v>
+      </c>
+      <c r="H54" s="12">
+        <v>1</v>
+      </c>
+      <c r="I54" s="12">
+        <v>2</v>
+      </c>
+      <c r="J54" s="12">
+        <v>2</v>
+      </c>
+      <c r="K54" s="12">
+        <v>1</v>
+      </c>
+      <c r="L54" s="12">
+        <v>1</v>
+      </c>
       <c r="M54" s="12">
         <v>6</v>
       </c>
@@ -5651,16 +6009,36 @@
       <c r="B55" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
+      <c r="C55" s="12">
+        <v>0</v>
+      </c>
+      <c r="D55" s="12">
+        <v>0</v>
+      </c>
+      <c r="E55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0</v>
+      </c>
+      <c r="G55" s="12">
+        <v>0</v>
+      </c>
+      <c r="H55" s="12">
+        <v>1</v>
+      </c>
+      <c r="I55" s="12">
+        <v>2</v>
+      </c>
+      <c r="J55" s="12">
+        <v>3</v>
+      </c>
+      <c r="K55" s="12">
+        <v>2</v>
+      </c>
+      <c r="L55" s="12">
+        <v>1</v>
+      </c>
       <c r="M55" s="13">
         <v>8</v>
       </c>
@@ -5669,16 +6047,36 @@
       <c r="B56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
+      <c r="C56" s="12">
+        <v>0</v>
+      </c>
+      <c r="D56" s="12">
+        <v>0</v>
+      </c>
+      <c r="E56" s="12">
+        <v>0</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0</v>
+      </c>
+      <c r="G56" s="12">
+        <v>0</v>
+      </c>
+      <c r="H56" s="12">
+        <v>1</v>
+      </c>
+      <c r="I56" s="12">
+        <v>2</v>
+      </c>
+      <c r="J56" s="12">
+        <v>3</v>
+      </c>
+      <c r="K56" s="12">
+        <v>2</v>
+      </c>
+      <c r="L56" s="12">
+        <v>1</v>
+      </c>
       <c r="M56" s="13">
         <v>8</v>
       </c>
@@ -5708,7 +6106,7 @@
       </c>
       <c r="C58" s="70">
         <f>SUM(C48:L55)</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D58" s="74"/>
       <c r="E58" s="74"/>
@@ -5727,7 +6125,7 @@
       </c>
       <c r="C59" s="70">
         <f>SUM(C57,-(C58))</f>
-        <v>60</v>
+        <v>-8</v>
       </c>
       <c r="D59" s="76"/>
       <c r="E59" s="77"/>
@@ -5798,16 +6196,36 @@
       <c r="B63" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="12"/>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
-      <c r="L63" s="12"/>
+      <c r="C63" s="12">
+        <v>2</v>
+      </c>
+      <c r="D63" s="12">
+        <v>2</v>
+      </c>
+      <c r="E63" s="12">
+        <v>2</v>
+      </c>
+      <c r="F63" s="12">
+        <v>2</v>
+      </c>
+      <c r="G63" s="12">
+        <v>2</v>
+      </c>
+      <c r="H63" s="12">
+        <v>0</v>
+      </c>
+      <c r="I63" s="12">
+        <v>0</v>
+      </c>
+      <c r="J63" s="12">
+        <v>0</v>
+      </c>
+      <c r="K63" s="12">
+        <v>0</v>
+      </c>
+      <c r="L63" s="12">
+        <v>0</v>
+      </c>
       <c r="M63" s="12">
         <v>10</v>
       </c>
@@ -5816,16 +6234,36 @@
       <c r="B64" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="12"/>
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
-      <c r="L64" s="12"/>
+      <c r="C64" s="12">
+        <v>2</v>
+      </c>
+      <c r="D64" s="12">
+        <v>2</v>
+      </c>
+      <c r="E64" s="12">
+        <v>2</v>
+      </c>
+      <c r="F64" s="12">
+        <v>2</v>
+      </c>
+      <c r="G64" s="12">
+        <v>2</v>
+      </c>
+      <c r="H64" s="12">
+        <v>0</v>
+      </c>
+      <c r="I64" s="12">
+        <v>0</v>
+      </c>
+      <c r="J64" s="12">
+        <v>0</v>
+      </c>
+      <c r="K64" s="12">
+        <v>0</v>
+      </c>
+      <c r="L64" s="12">
+        <v>0</v>
+      </c>
       <c r="M64" s="12">
         <v>10</v>
       </c>
@@ -5834,16 +6272,36 @@
       <c r="B65" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
-      <c r="I65" s="12"/>
-      <c r="J65" s="12"/>
-      <c r="K65" s="12"/>
-      <c r="L65" s="12"/>
+      <c r="C65" s="12">
+        <v>2</v>
+      </c>
+      <c r="D65" s="12">
+        <v>2</v>
+      </c>
+      <c r="E65" s="12">
+        <v>2</v>
+      </c>
+      <c r="F65" s="12">
+        <v>2</v>
+      </c>
+      <c r="G65" s="12">
+        <v>2</v>
+      </c>
+      <c r="H65" s="12">
+        <v>0</v>
+      </c>
+      <c r="I65" s="12">
+        <v>0</v>
+      </c>
+      <c r="J65" s="12">
+        <v>0</v>
+      </c>
+      <c r="K65" s="12">
+        <v>0</v>
+      </c>
+      <c r="L65" s="12">
+        <v>0</v>
+      </c>
       <c r="M65" s="12">
         <v>10</v>
       </c>
@@ -5852,16 +6310,36 @@
       <c r="B66" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
-      <c r="I66" s="12"/>
-      <c r="J66" s="12"/>
-      <c r="K66" s="12"/>
-      <c r="L66" s="12"/>
+      <c r="C66" s="12">
+        <v>0</v>
+      </c>
+      <c r="D66" s="12">
+        <v>0</v>
+      </c>
+      <c r="E66" s="12">
+        <v>1</v>
+      </c>
+      <c r="F66" s="12">
+        <v>2</v>
+      </c>
+      <c r="G66" s="12">
+        <v>3</v>
+      </c>
+      <c r="H66" s="12">
+        <v>3</v>
+      </c>
+      <c r="I66" s="12">
+        <v>1</v>
+      </c>
+      <c r="J66" s="12">
+        <v>1</v>
+      </c>
+      <c r="K66" s="12">
+        <v>0</v>
+      </c>
+      <c r="L66" s="12">
+        <v>0</v>
+      </c>
       <c r="M66" s="12">
         <v>10</v>
       </c>
@@ -5870,16 +6348,36 @@
       <c r="B67" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
-      <c r="J67" s="12"/>
-      <c r="K67" s="12"/>
-      <c r="L67" s="12"/>
+      <c r="C67" s="12">
+        <v>0</v>
+      </c>
+      <c r="D67" s="12">
+        <v>0</v>
+      </c>
+      <c r="E67" s="12">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="12">
+        <v>0</v>
+      </c>
+      <c r="H67" s="12">
+        <v>0</v>
+      </c>
+      <c r="I67" s="12">
+        <v>1</v>
+      </c>
+      <c r="J67" s="12">
+        <v>1</v>
+      </c>
+      <c r="K67" s="12">
+        <v>1</v>
+      </c>
+      <c r="L67" s="12">
+        <v>1</v>
+      </c>
       <c r="M67" s="12">
         <v>5</v>
       </c>
@@ -5888,16 +6386,36 @@
       <c r="B68" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="12"/>
-      <c r="I68" s="12"/>
-      <c r="J68" s="12"/>
-      <c r="K68" s="12"/>
-      <c r="L68" s="12"/>
+      <c r="C68" s="12">
+        <v>0</v>
+      </c>
+      <c r="D68" s="12">
+        <v>0</v>
+      </c>
+      <c r="E68" s="12">
+        <v>0</v>
+      </c>
+      <c r="F68" s="12">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
+        <v>0</v>
+      </c>
+      <c r="H68" s="12">
+        <v>0</v>
+      </c>
+      <c r="I68" s="12">
+        <v>1</v>
+      </c>
+      <c r="J68" s="12">
+        <v>1</v>
+      </c>
+      <c r="K68" s="12">
+        <v>1</v>
+      </c>
+      <c r="L68" s="12">
+        <v>1</v>
+      </c>
       <c r="M68" s="12">
         <v>5</v>
       </c>
@@ -5906,16 +6424,36 @@
       <c r="B69" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="12"/>
-      <c r="I69" s="12"/>
-      <c r="J69" s="12"/>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
+      <c r="C69" s="12">
+        <v>0</v>
+      </c>
+      <c r="D69" s="12">
+        <v>0</v>
+      </c>
+      <c r="E69" s="12">
+        <v>0</v>
+      </c>
+      <c r="F69" s="12">
+        <v>0</v>
+      </c>
+      <c r="G69" s="12">
+        <v>0</v>
+      </c>
+      <c r="H69" s="12">
+        <v>0</v>
+      </c>
+      <c r="I69" s="12">
+        <v>2</v>
+      </c>
+      <c r="J69" s="12">
+        <v>2</v>
+      </c>
+      <c r="K69" s="12">
+        <v>3</v>
+      </c>
+      <c r="L69" s="12">
+        <v>2</v>
+      </c>
       <c r="M69" s="12">
         <v>10</v>
       </c>
@@ -5924,16 +6462,36 @@
       <c r="B70" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-      <c r="K70" s="14"/>
-      <c r="L70" s="14"/>
+      <c r="C70" s="12">
+        <v>0</v>
+      </c>
+      <c r="D70" s="14">
+        <v>0</v>
+      </c>
+      <c r="E70" s="14">
+        <v>0</v>
+      </c>
+      <c r="F70" s="14">
+        <v>0</v>
+      </c>
+      <c r="G70" s="14">
+        <v>0</v>
+      </c>
+      <c r="H70" s="14">
+        <v>0</v>
+      </c>
+      <c r="I70" s="14">
+        <v>1</v>
+      </c>
+      <c r="J70" s="14">
+        <v>2</v>
+      </c>
+      <c r="K70" s="14">
+        <v>2</v>
+      </c>
+      <c r="L70" s="14">
+        <v>2</v>
+      </c>
       <c r="M70" s="14">
         <v>5</v>
       </c>
@@ -5963,7 +6521,7 @@
       </c>
       <c r="C72" s="70">
         <f>SUM(C63:L70)</f>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D72" s="74"/>
       <c r="E72" s="74"/>
@@ -5982,7 +6540,7 @@
       </c>
       <c r="C73" s="70">
         <f>SUM(C71,-(C72))</f>
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D73" s="76"/>
       <c r="E73" s="77"/>
@@ -6053,16 +6611,36 @@
       <c r="B77" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
-      <c r="H77" s="12"/>
-      <c r="I77" s="12"/>
-      <c r="J77" s="12"/>
-      <c r="K77" s="12"/>
-      <c r="L77" s="12"/>
+      <c r="C77" s="12">
+        <v>3</v>
+      </c>
+      <c r="D77" s="12">
+        <v>2</v>
+      </c>
+      <c r="E77" s="12">
+        <v>1</v>
+      </c>
+      <c r="F77" s="12">
+        <v>1</v>
+      </c>
+      <c r="G77" s="12">
+        <v>1</v>
+      </c>
+      <c r="H77" s="12">
+        <v>0</v>
+      </c>
+      <c r="I77" s="12">
+        <v>0</v>
+      </c>
+      <c r="J77" s="12">
+        <v>0</v>
+      </c>
+      <c r="K77" s="12">
+        <v>0</v>
+      </c>
+      <c r="L77" s="12">
+        <v>0</v>
+      </c>
       <c r="M77" s="12">
         <v>10</v>
       </c>
@@ -6071,16 +6649,36 @@
       <c r="B78" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="12"/>
-      <c r="I78" s="12"/>
-      <c r="J78" s="12"/>
-      <c r="K78" s="12"/>
-      <c r="L78" s="12"/>
+      <c r="C78" s="12">
+        <v>3</v>
+      </c>
+      <c r="D78" s="12">
+        <v>2</v>
+      </c>
+      <c r="E78" s="12">
+        <v>1</v>
+      </c>
+      <c r="F78" s="12">
+        <v>1</v>
+      </c>
+      <c r="G78" s="12">
+        <v>1</v>
+      </c>
+      <c r="H78" s="12">
+        <v>0</v>
+      </c>
+      <c r="I78" s="12">
+        <v>0</v>
+      </c>
+      <c r="J78" s="12">
+        <v>0</v>
+      </c>
+      <c r="K78" s="12">
+        <v>0</v>
+      </c>
+      <c r="L78" s="12">
+        <v>0</v>
+      </c>
       <c r="M78" s="12">
         <v>10</v>
       </c>
@@ -6089,16 +6687,36 @@
       <c r="B79" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C79" s="12"/>
-      <c r="D79" s="12"/>
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="12"/>
-      <c r="I79" s="12"/>
-      <c r="J79" s="12"/>
-      <c r="K79" s="12"/>
-      <c r="L79" s="12"/>
+      <c r="C79" s="12">
+        <v>0</v>
+      </c>
+      <c r="D79" s="12">
+        <v>2</v>
+      </c>
+      <c r="E79" s="12">
+        <v>2</v>
+      </c>
+      <c r="F79" s="12">
+        <v>2</v>
+      </c>
+      <c r="G79" s="12">
+        <v>1</v>
+      </c>
+      <c r="H79" s="12">
+        <v>0</v>
+      </c>
+      <c r="I79" s="12">
+        <v>0</v>
+      </c>
+      <c r="J79" s="12">
+        <v>0</v>
+      </c>
+      <c r="K79" s="12">
+        <v>0</v>
+      </c>
+      <c r="L79" s="12">
+        <v>0</v>
+      </c>
       <c r="M79" s="12">
         <v>6</v>
       </c>
@@ -6107,16 +6725,36 @@
       <c r="B80" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="12"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="12"/>
-      <c r="I80" s="12"/>
-      <c r="J80" s="12"/>
-      <c r="K80" s="12"/>
-      <c r="L80" s="12"/>
+      <c r="C80" s="12">
+        <v>0</v>
+      </c>
+      <c r="D80" s="12">
+        <v>2</v>
+      </c>
+      <c r="E80" s="12">
+        <v>2</v>
+      </c>
+      <c r="F80" s="12">
+        <v>2</v>
+      </c>
+      <c r="G80" s="12">
+        <v>1</v>
+      </c>
+      <c r="H80" s="12">
+        <v>0</v>
+      </c>
+      <c r="I80" s="12">
+        <v>0</v>
+      </c>
+      <c r="J80" s="12">
+        <v>0</v>
+      </c>
+      <c r="K80" s="12">
+        <v>0</v>
+      </c>
+      <c r="L80" s="12">
+        <v>0</v>
+      </c>
       <c r="M80" s="12">
         <v>6</v>
       </c>
@@ -6125,16 +6763,36 @@
       <c r="B81" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12"/>
-      <c r="G81" s="12"/>
-      <c r="H81" s="12"/>
-      <c r="I81" s="12"/>
-      <c r="J81" s="12"/>
-      <c r="K81" s="12"/>
-      <c r="L81" s="12"/>
+      <c r="C81" s="12">
+        <v>0</v>
+      </c>
+      <c r="D81" s="12">
+        <v>2</v>
+      </c>
+      <c r="E81" s="12">
+        <v>2</v>
+      </c>
+      <c r="F81" s="12">
+        <v>2</v>
+      </c>
+      <c r="G81" s="12">
+        <v>1</v>
+      </c>
+      <c r="H81" s="12">
+        <v>0</v>
+      </c>
+      <c r="I81" s="12">
+        <v>0</v>
+      </c>
+      <c r="J81" s="12">
+        <v>0</v>
+      </c>
+      <c r="K81" s="12">
+        <v>0</v>
+      </c>
+      <c r="L81" s="12">
+        <v>0</v>
+      </c>
       <c r="M81" s="12">
         <v>8</v>
       </c>
@@ -6143,16 +6801,36 @@
       <c r="B82" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
-      <c r="G82" s="12"/>
-      <c r="H82" s="12"/>
-      <c r="I82" s="12"/>
-      <c r="J82" s="12"/>
-      <c r="K82" s="12"/>
-      <c r="L82" s="12"/>
+      <c r="C82" s="12">
+        <v>0</v>
+      </c>
+      <c r="D82" s="12">
+        <v>2</v>
+      </c>
+      <c r="E82" s="12">
+        <v>2</v>
+      </c>
+      <c r="F82" s="12">
+        <v>2</v>
+      </c>
+      <c r="G82" s="12">
+        <v>1</v>
+      </c>
+      <c r="H82" s="12">
+        <v>0</v>
+      </c>
+      <c r="I82" s="12">
+        <v>0</v>
+      </c>
+      <c r="J82" s="12">
+        <v>0</v>
+      </c>
+      <c r="K82" s="12">
+        <v>0</v>
+      </c>
+      <c r="L82" s="12">
+        <v>0</v>
+      </c>
       <c r="M82" s="12">
         <v>8</v>
       </c>
@@ -6161,16 +6839,36 @@
       <c r="B83" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-      <c r="I83" s="12"/>
-      <c r="J83" s="12"/>
-      <c r="K83" s="12"/>
-      <c r="L83" s="12"/>
+      <c r="C83" s="12">
+        <v>0</v>
+      </c>
+      <c r="D83" s="12">
+        <v>2</v>
+      </c>
+      <c r="E83" s="12">
+        <v>2</v>
+      </c>
+      <c r="F83" s="12">
+        <v>2</v>
+      </c>
+      <c r="G83" s="12">
+        <v>1</v>
+      </c>
+      <c r="H83" s="12">
+        <v>0</v>
+      </c>
+      <c r="I83" s="12">
+        <v>0</v>
+      </c>
+      <c r="J83" s="12">
+        <v>0</v>
+      </c>
+      <c r="K83" s="12">
+        <v>0</v>
+      </c>
+      <c r="L83" s="12">
+        <v>0</v>
+      </c>
       <c r="M83" s="12">
         <v>8</v>
       </c>
@@ -6179,16 +6877,36 @@
       <c r="B84" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
-      <c r="J84" s="12"/>
-      <c r="K84" s="12"/>
-      <c r="L84" s="12"/>
+      <c r="C84" s="12">
+        <v>0</v>
+      </c>
+      <c r="D84" s="12">
+        <v>0</v>
+      </c>
+      <c r="E84" s="12">
+        <v>0</v>
+      </c>
+      <c r="F84" s="12">
+        <v>2</v>
+      </c>
+      <c r="G84" s="12">
+        <v>2</v>
+      </c>
+      <c r="H84" s="12">
+        <v>0</v>
+      </c>
+      <c r="I84" s="12">
+        <v>0</v>
+      </c>
+      <c r="J84" s="12">
+        <v>0</v>
+      </c>
+      <c r="K84" s="12">
+        <v>0</v>
+      </c>
+      <c r="L84" s="12">
+        <v>0</v>
+      </c>
       <c r="M84" s="12">
         <v>4</v>
       </c>
@@ -6218,7 +6936,7 @@
       </c>
       <c r="C86" s="70">
         <f>SUM(C77:L84)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="D86" s="74"/>
       <c r="E86" s="74"/>
@@ -6237,7 +6955,7 @@
       </c>
       <c r="C87" s="70">
         <f>SUM(C85,-(C86))</f>
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D87" s="76"/>
       <c r="E87" s="77"/>
@@ -6273,7 +6991,7 @@
   <dimension ref="A1:CN92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6304,14 +7022,17 @@
     <col min="44" max="44" width="3.42578125" style="1" customWidth="1"/>
     <col min="45" max="45" width="3.140625" style="1" customWidth="1"/>
     <col min="46" max="46" width="3.42578125" style="1" customWidth="1"/>
-    <col min="47" max="47" width="3.140625" style="1" customWidth="1"/>
-    <col min="48" max="48" width="4.28515625" style="1" customWidth="1"/>
+    <col min="47" max="48" width="3.140625" style="1" customWidth="1"/>
     <col min="49" max="49" width="3.85546875" style="1" customWidth="1"/>
-    <col min="50" max="50" width="5.140625" style="1" customWidth="1"/>
-    <col min="51" max="57" width="4.28515625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="4.5703125" style="1" customWidth="1"/>
-    <col min="59" max="59" width="4.28515625" style="1" customWidth="1"/>
-    <col min="60" max="66" width="4.5703125" style="1" customWidth="1"/>
+    <col min="50" max="52" width="3.140625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="3.28515625" style="1" customWidth="1"/>
+    <col min="54" max="55" width="3.140625" style="1" customWidth="1"/>
+    <col min="56" max="56" width="4.140625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="4.28515625" style="1" customWidth="1"/>
+    <col min="58" max="59" width="3.140625" style="1" customWidth="1"/>
+    <col min="60" max="60" width="3.28515625" style="1" customWidth="1"/>
+    <col min="61" max="62" width="3.140625" style="1" customWidth="1"/>
+    <col min="63" max="66" width="4.5703125" style="1" customWidth="1"/>
     <col min="67" max="67" width="3.28515625" style="1" customWidth="1"/>
     <col min="68" max="68" width="4.5703125" style="1" customWidth="1"/>
     <col min="69" max="69" width="2.85546875" style="1" customWidth="1"/>
@@ -8192,12 +8913,12 @@
       <c r="C17" s="91">
         <v>2</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="108"/>
+      <c r="E17" s="109"/>
+      <c r="F17" s="109"/>
+      <c r="G17" s="109"/>
       <c r="H17" s="33"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -9393,12 +10114,14 @@
         <v>94</v>
       </c>
       <c r="E29" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="82">
         <v>44440</v>
       </c>
-      <c r="G29" s="82"/>
+      <c r="G29" s="82">
+        <v>44446</v>
+      </c>
       <c r="H29" s="34"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
@@ -9493,12 +10216,14 @@
         <v>93</v>
       </c>
       <c r="E30" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="82">
         <v>44440</v>
       </c>
-      <c r="G30" s="82"/>
+      <c r="G30" s="82">
+        <v>44446</v>
+      </c>
       <c r="H30" s="34"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
@@ -9593,12 +10318,14 @@
         <v>99</v>
       </c>
       <c r="E31" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="82">
         <v>44440</v>
       </c>
-      <c r="G31" s="82"/>
+      <c r="G31" s="82">
+        <v>44446</v>
+      </c>
       <c r="H31" s="34"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
@@ -9693,12 +10420,14 @@
         <v>100</v>
       </c>
       <c r="E32" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="82">
         <v>44440</v>
       </c>
-      <c r="G32" s="82"/>
+      <c r="G32" s="82">
+        <v>44446</v>
+      </c>
       <c r="H32" s="34"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
@@ -9793,12 +10522,14 @@
         <v>102</v>
       </c>
       <c r="E33" s="81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="82">
         <v>44440</v>
       </c>
-      <c r="G33" s="82"/>
+      <c r="G33" s="82">
+        <v>44446</v>
+      </c>
       <c r="H33" s="34"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
@@ -9989,10 +10720,14 @@
         <v>101</v>
       </c>
       <c r="E35" s="81">
-        <v>0</v>
-      </c>
-      <c r="F35" s="82"/>
-      <c r="G35" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G35" s="82">
+        <v>44448</v>
+      </c>
       <c r="H35" s="34"/>
       <c r="I35" s="27"/>
       <c r="J35" s="27"/>
@@ -10033,7 +10768,7 @@
       <c r="AS35" s="99"/>
       <c r="AT35" s="99"/>
       <c r="AU35" s="99"/>
-      <c r="AV35" s="99"/>
+      <c r="AV35" s="47"/>
       <c r="AW35" s="8"/>
       <c r="AX35" s="8"/>
       <c r="AY35" s="8"/>
@@ -10087,10 +10822,14 @@
         <v>111</v>
       </c>
       <c r="E36" s="81">
-        <v>0</v>
-      </c>
-      <c r="F36" s="82"/>
-      <c r="G36" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F36" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G36" s="82">
+        <v>44448</v>
+      </c>
       <c r="H36" s="34"/>
       <c r="I36" s="27"/>
       <c r="J36" s="27"/>
@@ -10131,7 +10870,7 @@
       <c r="AS36" s="99"/>
       <c r="AT36" s="99"/>
       <c r="AU36" s="99"/>
-      <c r="AV36" s="99"/>
+      <c r="AV36" s="47"/>
       <c r="AW36" s="8"/>
       <c r="AX36" s="8"/>
       <c r="AY36" s="8"/>
@@ -10185,10 +10924,14 @@
         <v>112</v>
       </c>
       <c r="E37" s="81">
-        <v>0</v>
-      </c>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F37" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G37" s="82">
+        <v>44448</v>
+      </c>
       <c r="H37" s="34"/>
       <c r="I37" s="27"/>
       <c r="J37" s="27"/>
@@ -10229,7 +10972,7 @@
       <c r="AS37" s="99"/>
       <c r="AT37" s="99"/>
       <c r="AU37" s="99"/>
-      <c r="AV37" s="99"/>
+      <c r="AV37" s="47"/>
       <c r="AW37" s="8"/>
       <c r="AX37" s="8"/>
       <c r="AY37" s="8"/>
@@ -10283,10 +11026,14 @@
         <v>103</v>
       </c>
       <c r="E38" s="81">
-        <v>0</v>
-      </c>
-      <c r="F38" s="82"/>
-      <c r="G38" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G38" s="82">
+        <v>44448</v>
+      </c>
       <c r="H38" s="34"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
@@ -10327,7 +11074,7 @@
       <c r="AS38" s="99"/>
       <c r="AT38" s="99"/>
       <c r="AU38" s="99"/>
-      <c r="AV38" s="99"/>
+      <c r="AV38" s="47"/>
       <c r="AW38" s="8"/>
       <c r="AX38" s="8"/>
       <c r="AY38" s="8"/>
@@ -10381,10 +11128,14 @@
         <v>104</v>
       </c>
       <c r="E39" s="81">
-        <v>0</v>
-      </c>
-      <c r="F39" s="82"/>
-      <c r="G39" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F39" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G39" s="82">
+        <v>44448</v>
+      </c>
       <c r="H39" s="34"/>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -10425,7 +11176,7 @@
       <c r="AS39" s="99"/>
       <c r="AT39" s="99"/>
       <c r="AU39" s="99"/>
-      <c r="AV39" s="99"/>
+      <c r="AV39" s="47"/>
       <c r="AW39" s="8"/>
       <c r="AX39" s="8"/>
       <c r="AY39" s="8"/>
@@ -10479,10 +11230,14 @@
         <v>144</v>
       </c>
       <c r="E40" s="81">
-        <v>0</v>
-      </c>
-      <c r="F40" s="82"/>
-      <c r="G40" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F40" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G40" s="82">
+        <v>44448</v>
+      </c>
       <c r="H40" s="34"/>
       <c r="I40" s="27"/>
       <c r="J40" s="27"/>
@@ -10523,7 +11278,7 @@
       <c r="AS40" s="99"/>
       <c r="AT40" s="99"/>
       <c r="AU40" s="99"/>
-      <c r="AV40" s="99"/>
+      <c r="AV40" s="47"/>
       <c r="AW40" s="8"/>
       <c r="AX40" s="8"/>
       <c r="AY40" s="8"/>
@@ -10577,10 +11332,14 @@
         <v>145</v>
       </c>
       <c r="E41" s="81">
-        <v>0</v>
-      </c>
-      <c r="F41" s="82"/>
-      <c r="G41" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F41" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G41" s="82">
+        <v>44448</v>
+      </c>
       <c r="H41" s="34"/>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
@@ -10621,7 +11380,7 @@
       <c r="AS41" s="99"/>
       <c r="AT41" s="99"/>
       <c r="AU41" s="99"/>
-      <c r="AV41" s="99"/>
+      <c r="AV41" s="47"/>
       <c r="AW41" s="8"/>
       <c r="AX41" s="8"/>
       <c r="AY41" s="8"/>
@@ -10675,10 +11434,14 @@
         <v>146</v>
       </c>
       <c r="E42" s="81">
-        <v>0</v>
-      </c>
-      <c r="F42" s="82"/>
-      <c r="G42" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F42" s="82">
+        <v>44441</v>
+      </c>
+      <c r="G42" s="82">
+        <v>44448</v>
+      </c>
       <c r="H42" s="34"/>
       <c r="I42" s="27"/>
       <c r="J42" s="27"/>
@@ -10719,7 +11482,7 @@
       <c r="AS42" s="99"/>
       <c r="AT42" s="99"/>
       <c r="AU42" s="99"/>
-      <c r="AV42" s="99"/>
+      <c r="AV42" s="47"/>
       <c r="AW42" s="8"/>
       <c r="AX42" s="8"/>
       <c r="AY42" s="8"/>
@@ -10773,10 +11536,14 @@
         <v>106</v>
       </c>
       <c r="E43" s="81">
-        <v>0</v>
-      </c>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F43" s="82">
+        <v>44447</v>
+      </c>
+      <c r="G43" s="82">
+        <v>44449</v>
+      </c>
       <c r="H43" s="34"/>
       <c r="I43" s="27"/>
       <c r="J43" s="27"/>
@@ -10814,7 +11581,7 @@
       <c r="AP43" s="8"/>
       <c r="AQ43" s="8"/>
       <c r="AR43" s="8"/>
-      <c r="AS43" s="99"/>
+      <c r="AS43" s="47"/>
       <c r="AT43" s="99"/>
       <c r="AU43" s="99"/>
       <c r="AV43" s="99"/>
@@ -10871,10 +11638,14 @@
         <v>105</v>
       </c>
       <c r="E44" s="81">
-        <v>0</v>
-      </c>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F44" s="82">
+        <v>44447</v>
+      </c>
+      <c r="G44" s="82">
+        <v>44449</v>
+      </c>
       <c r="H44" s="34"/>
       <c r="I44" s="27"/>
       <c r="J44" s="27"/>
@@ -10912,7 +11683,7 @@
       <c r="AP44" s="8"/>
       <c r="AQ44" s="8"/>
       <c r="AR44" s="8"/>
-      <c r="AS44" s="99"/>
+      <c r="AS44" s="47"/>
       <c r="AT44" s="99"/>
       <c r="AU44" s="99"/>
       <c r="AV44" s="99"/>
@@ -10969,10 +11740,14 @@
         <v>109</v>
       </c>
       <c r="E45" s="81">
-        <v>0</v>
-      </c>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F45" s="82">
+        <v>44447</v>
+      </c>
+      <c r="G45" s="82">
+        <v>44449</v>
+      </c>
       <c r="H45" s="34"/>
       <c r="I45" s="27"/>
       <c r="J45" s="27"/>
@@ -11010,7 +11785,7 @@
       <c r="AP45" s="8"/>
       <c r="AQ45" s="8"/>
       <c r="AR45" s="8"/>
-      <c r="AS45" s="99"/>
+      <c r="AS45" s="47"/>
       <c r="AT45" s="99"/>
       <c r="AU45" s="99"/>
       <c r="AV45" s="99"/>
@@ -11063,12 +11838,12 @@
       <c r="C46" s="91">
         <v>4</v>
       </c>
-      <c r="D46" s="108" t="s">
+      <c r="D46" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E46" s="108"/>
-      <c r="F46" s="108"/>
-      <c r="G46" s="108"/>
+      <c r="E46" s="109"/>
+      <c r="F46" s="109"/>
+      <c r="G46" s="109"/>
       <c r="H46" s="34"/>
       <c r="I46" s="27"/>
       <c r="J46" s="27"/>
@@ -11163,10 +11938,14 @@
         <v>154</v>
       </c>
       <c r="E47" s="81">
-        <v>0</v>
-      </c>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F47" s="82">
+        <v>44447</v>
+      </c>
+      <c r="G47" s="82">
+        <v>44449</v>
+      </c>
       <c r="H47" s="34"/>
       <c r="I47" s="27"/>
       <c r="J47" s="27"/>
@@ -11451,10 +12230,14 @@
         <v>113</v>
       </c>
       <c r="E50" s="81">
-        <v>0</v>
-      </c>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F50" s="82">
+        <v>44452</v>
+      </c>
+      <c r="G50" s="82">
+        <v>44456</v>
+      </c>
       <c r="H50" s="34"/>
       <c r="I50" s="27"/>
       <c r="J50" s="27"/>
@@ -11502,7 +12285,7 @@
       <c r="AZ50" s="99"/>
       <c r="BA50" s="99"/>
       <c r="BB50" s="99"/>
-      <c r="BC50" s="8"/>
+      <c r="BC50" s="99"/>
       <c r="BD50" s="8"/>
       <c r="BE50" s="8"/>
       <c r="BF50" s="8"/>
@@ -11549,10 +12332,14 @@
         <v>115</v>
       </c>
       <c r="E51" s="81">
-        <v>0</v>
-      </c>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="82">
+        <v>44452</v>
+      </c>
+      <c r="G51" s="82">
+        <v>44456</v>
+      </c>
       <c r="H51" s="34"/>
       <c r="I51" s="27"/>
       <c r="J51" s="27"/>
@@ -11600,7 +12387,7 @@
       <c r="AZ51" s="99"/>
       <c r="BA51" s="99"/>
       <c r="BB51" s="99"/>
-      <c r="BC51" s="8"/>
+      <c r="BC51" s="99"/>
       <c r="BD51" s="8"/>
       <c r="BE51" s="8"/>
       <c r="BF51" s="8"/>
@@ -11647,10 +12434,14 @@
         <v>114</v>
       </c>
       <c r="E52" s="81">
-        <v>0</v>
-      </c>
-      <c r="F52" s="82"/>
-      <c r="G52" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F52" s="82">
+        <v>44452</v>
+      </c>
+      <c r="G52" s="82">
+        <v>44456</v>
+      </c>
       <c r="H52" s="34"/>
       <c r="I52" s="27"/>
       <c r="J52" s="27"/>
@@ -11698,7 +12489,7 @@
       <c r="AZ52" s="99"/>
       <c r="BA52" s="99"/>
       <c r="BB52" s="99"/>
-      <c r="BC52" s="8"/>
+      <c r="BC52" s="99"/>
       <c r="BD52" s="8"/>
       <c r="BE52" s="8"/>
       <c r="BF52" s="8"/>
@@ -11841,10 +12632,14 @@
         <v>116</v>
       </c>
       <c r="E54" s="81">
-        <v>0</v>
-      </c>
-      <c r="F54" s="82"/>
-      <c r="G54" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F54" s="82">
+        <v>44454</v>
+      </c>
+      <c r="G54" s="82">
+        <v>44460</v>
+      </c>
       <c r="H54" s="33"/>
       <c r="I54" s="27"/>
       <c r="J54" s="27"/>
@@ -11939,10 +12734,14 @@
         <v>147</v>
       </c>
       <c r="E55" s="81">
-        <v>0</v>
-      </c>
-      <c r="F55" s="82"/>
-      <c r="G55" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F55" s="82">
+        <v>44454</v>
+      </c>
+      <c r="G55" s="82">
+        <v>44460</v>
+      </c>
       <c r="H55" s="33"/>
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
@@ -12037,10 +12836,14 @@
         <v>118</v>
       </c>
       <c r="E56" s="81">
-        <v>0</v>
-      </c>
-      <c r="F56" s="82"/>
-      <c r="G56" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F56" s="82">
+        <v>44454</v>
+      </c>
+      <c r="G56" s="82">
+        <v>44460</v>
+      </c>
       <c r="H56" s="33"/>
       <c r="I56" s="27"/>
       <c r="J56" s="27"/>
@@ -12135,10 +12938,14 @@
         <v>117</v>
       </c>
       <c r="E57" s="81">
-        <v>0</v>
-      </c>
-      <c r="F57" s="82"/>
-      <c r="G57" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F57" s="82">
+        <v>44454</v>
+      </c>
+      <c r="G57" s="82">
+        <v>44460</v>
+      </c>
       <c r="H57" s="33"/>
       <c r="I57" s="27"/>
       <c r="J57" s="27"/>
@@ -12233,10 +13040,14 @@
         <v>119</v>
       </c>
       <c r="E58" s="81">
-        <v>0</v>
-      </c>
-      <c r="F58" s="82"/>
-      <c r="G58" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F58" s="82">
+        <v>44459</v>
+      </c>
+      <c r="G58" s="82">
+        <v>44463</v>
+      </c>
       <c r="H58" s="33"/>
       <c r="I58" s="27"/>
       <c r="J58" s="27"/>
@@ -12331,10 +13142,14 @@
         <v>121</v>
       </c>
       <c r="E59" s="81">
-        <v>0</v>
-      </c>
-      <c r="F59" s="82"/>
-      <c r="G59" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F59" s="82">
+        <v>44459</v>
+      </c>
+      <c r="G59" s="82">
+        <v>44463</v>
+      </c>
       <c r="H59" s="33"/>
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
@@ -12429,10 +13244,14 @@
         <v>120</v>
       </c>
       <c r="E60" s="81">
-        <v>0</v>
-      </c>
-      <c r="F60" s="82"/>
-      <c r="G60" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F60" s="82">
+        <v>44459</v>
+      </c>
+      <c r="G60" s="82">
+        <v>44463</v>
+      </c>
       <c r="H60" s="33"/>
       <c r="I60" s="27"/>
       <c r="J60" s="27"/>
@@ -12527,10 +13346,14 @@
         <v>122</v>
       </c>
       <c r="E61" s="81">
-        <v>0</v>
-      </c>
-      <c r="F61" s="82"/>
-      <c r="G61" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F61" s="82">
+        <v>44459</v>
+      </c>
+      <c r="G61" s="82">
+        <v>44463</v>
+      </c>
       <c r="H61" s="33"/>
       <c r="I61" s="27"/>
       <c r="J61" s="27"/>
@@ -12621,12 +13444,12 @@
       <c r="C62" s="91">
         <v>3</v>
       </c>
-      <c r="D62" s="108" t="s">
+      <c r="D62" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E62" s="108"/>
-      <c r="F62" s="108"/>
-      <c r="G62" s="108"/>
+      <c r="E62" s="109"/>
+      <c r="F62" s="109"/>
+      <c r="G62" s="109"/>
       <c r="H62" s="33"/>
       <c r="I62" s="27"/>
       <c r="J62" s="27"/>
@@ -12721,10 +13544,14 @@
         <v>154</v>
       </c>
       <c r="E63" s="81">
-        <v>0</v>
-      </c>
-      <c r="F63" s="82"/>
-      <c r="G63" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F63" s="82">
+        <v>44461</v>
+      </c>
+      <c r="G63" s="82">
+        <v>44463</v>
+      </c>
       <c r="H63" s="33"/>
       <c r="I63" s="27"/>
       <c r="J63" s="27"/>
@@ -13009,10 +13836,14 @@
         <v>123</v>
       </c>
       <c r="E66" s="81">
-        <v>0</v>
-      </c>
-      <c r="F66" s="82"/>
-      <c r="G66" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F66" s="82">
+        <v>44466</v>
+      </c>
+      <c r="G66" s="82">
+        <v>44470</v>
+      </c>
       <c r="H66" s="33"/>
       <c r="I66" s="27"/>
       <c r="J66" s="27"/>
@@ -13107,10 +13938,14 @@
         <v>129</v>
       </c>
       <c r="E67" s="81">
-        <v>0</v>
-      </c>
-      <c r="F67" s="82"/>
-      <c r="G67" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F67" s="82">
+        <v>44466</v>
+      </c>
+      <c r="G67" s="82">
+        <v>44470</v>
+      </c>
       <c r="H67" s="33"/>
       <c r="I67" s="27"/>
       <c r="J67" s="27"/>
@@ -13205,10 +14040,14 @@
         <v>124</v>
       </c>
       <c r="E68" s="81">
-        <v>0</v>
-      </c>
-      <c r="F68" s="82"/>
-      <c r="G68" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F68" s="82">
+        <v>44466</v>
+      </c>
+      <c r="G68" s="82">
+        <v>44470</v>
+      </c>
       <c r="H68" s="33"/>
       <c r="I68" s="27"/>
       <c r="J68" s="27"/>
@@ -13303,10 +14142,14 @@
         <v>130</v>
       </c>
       <c r="E69" s="81">
-        <v>0</v>
-      </c>
-      <c r="F69" s="82"/>
-      <c r="G69" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F69" s="82">
+        <v>44466</v>
+      </c>
+      <c r="G69" s="82">
+        <v>44470</v>
+      </c>
       <c r="H69" s="33"/>
       <c r="I69" s="27"/>
       <c r="J69" s="27"/>
@@ -13401,10 +14244,14 @@
         <v>126</v>
       </c>
       <c r="E70" s="81">
-        <v>0</v>
-      </c>
-      <c r="F70" s="82"/>
-      <c r="G70" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F70" s="82">
+        <v>44468</v>
+      </c>
+      <c r="G70" s="82">
+        <v>44475</v>
+      </c>
       <c r="H70" s="33"/>
       <c r="I70" s="27"/>
       <c r="J70" s="27"/>
@@ -13499,10 +14346,14 @@
         <v>127</v>
       </c>
       <c r="E71" s="81">
-        <v>0</v>
-      </c>
-      <c r="F71" s="82"/>
-      <c r="G71" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F71" s="82">
+        <v>44468</v>
+      </c>
+      <c r="G71" s="82">
+        <v>44475</v>
+      </c>
       <c r="H71" s="33"/>
       <c r="I71" s="27"/>
       <c r="J71" s="27"/>
@@ -13597,10 +14448,14 @@
         <v>128</v>
       </c>
       <c r="E72" s="81">
-        <v>0</v>
-      </c>
-      <c r="F72" s="82"/>
-      <c r="G72" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F72" s="82">
+        <v>44468</v>
+      </c>
+      <c r="G72" s="82">
+        <v>44475</v>
+      </c>
       <c r="H72" s="33"/>
       <c r="I72" s="27"/>
       <c r="J72" s="27"/>
@@ -13695,10 +14550,14 @@
         <v>138</v>
       </c>
       <c r="E73" s="81">
-        <v>0</v>
-      </c>
-      <c r="F73" s="82"/>
-      <c r="G73" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F73" s="82">
+        <v>44468</v>
+      </c>
+      <c r="G73" s="82">
+        <v>44475</v>
+      </c>
       <c r="H73" s="33"/>
       <c r="I73" s="27"/>
       <c r="J73" s="27"/>
@@ -13793,10 +14652,14 @@
         <v>131</v>
       </c>
       <c r="E74" s="81">
-        <v>0</v>
-      </c>
-      <c r="F74" s="82"/>
-      <c r="G74" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F74" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G74" s="82">
+        <v>44477</v>
+      </c>
       <c r="H74" s="33"/>
       <c r="I74" s="27"/>
       <c r="J74" s="27"/>
@@ -13891,10 +14754,14 @@
         <v>132</v>
       </c>
       <c r="E75" s="81">
-        <v>0</v>
-      </c>
-      <c r="F75" s="82"/>
-      <c r="G75" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F75" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G75" s="82">
+        <v>44477</v>
+      </c>
       <c r="H75" s="33"/>
       <c r="I75" s="27"/>
       <c r="J75" s="27"/>
@@ -13989,10 +14856,14 @@
         <v>133</v>
       </c>
       <c r="E76" s="81">
-        <v>0</v>
-      </c>
-      <c r="F76" s="82"/>
-      <c r="G76" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F76" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G76" s="82">
+        <v>44477</v>
+      </c>
       <c r="H76" s="33"/>
       <c r="I76" s="27"/>
       <c r="J76" s="27"/>
@@ -14087,10 +14958,14 @@
         <v>134</v>
       </c>
       <c r="E77" s="81">
-        <v>0</v>
-      </c>
-      <c r="F77" s="82"/>
-      <c r="G77" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F77" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G77" s="82">
+        <v>44477</v>
+      </c>
       <c r="H77" s="33"/>
       <c r="I77" s="27"/>
       <c r="J77" s="27"/>
@@ -14181,12 +15056,12 @@
       <c r="C78" s="91">
         <v>2</v>
       </c>
-      <c r="D78" s="108" t="s">
+      <c r="D78" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E78" s="108"/>
-      <c r="F78" s="108"/>
-      <c r="G78" s="108"/>
+      <c r="E78" s="109"/>
+      <c r="F78" s="109"/>
+      <c r="G78" s="109"/>
       <c r="H78" s="33"/>
       <c r="I78" s="27"/>
       <c r="J78" s="27"/>
@@ -14281,10 +15156,14 @@
         <v>63</v>
       </c>
       <c r="E79" s="81">
-        <v>0</v>
-      </c>
-      <c r="F79" s="82"/>
-      <c r="G79" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F79" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G79" s="82">
+        <v>44478</v>
+      </c>
       <c r="H79" s="33"/>
       <c r="I79" s="27"/>
       <c r="J79" s="27"/>
@@ -14379,10 +15258,14 @@
         <v>136</v>
       </c>
       <c r="E80" s="81">
-        <v>0</v>
-      </c>
-      <c r="F80" s="82"/>
-      <c r="G80" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F80" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G80" s="82">
+        <v>44478</v>
+      </c>
       <c r="H80" s="33"/>
       <c r="I80" s="27"/>
       <c r="J80" s="27"/>
@@ -14477,10 +15360,14 @@
         <v>154</v>
       </c>
       <c r="E81" s="81">
-        <v>0</v>
-      </c>
-      <c r="F81" s="82"/>
-      <c r="G81" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F81" s="82">
+        <v>44474</v>
+      </c>
+      <c r="G81" s="82">
+        <v>44478</v>
+      </c>
       <c r="H81" s="33"/>
       <c r="I81" s="27"/>
       <c r="J81" s="27"/>
@@ -14574,7 +15461,7 @@
       </c>
       <c r="E82" s="107"/>
       <c r="F82" s="107"/>
-      <c r="G82" s="109"/>
+      <c r="G82" s="108"/>
       <c r="H82" s="30"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
@@ -14765,10 +15652,14 @@
         <v>16</v>
       </c>
       <c r="E84" s="81">
-        <v>0</v>
-      </c>
-      <c r="F84" s="82"/>
-      <c r="G84" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F84" s="82">
+        <v>44480</v>
+      </c>
+      <c r="G84" s="82">
+        <v>44484</v>
+      </c>
       <c r="H84" s="33"/>
       <c r="I84" s="8"/>
       <c r="J84" s="8"/>
@@ -14863,10 +15754,14 @@
         <v>135</v>
       </c>
       <c r="E85" s="81">
-        <v>0</v>
-      </c>
-      <c r="F85" s="82"/>
-      <c r="G85" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F85" s="82">
+        <v>44480</v>
+      </c>
+      <c r="G85" s="82">
+        <v>44484</v>
+      </c>
       <c r="H85" s="33"/>
       <c r="I85" s="8"/>
       <c r="J85" s="8"/>
@@ -14957,12 +15852,12 @@
       <c r="C86" s="91">
         <v>2</v>
       </c>
-      <c r="D86" s="108" t="s">
+      <c r="D86" s="109" t="s">
         <v>17</v>
       </c>
-      <c r="E86" s="108"/>
-      <c r="F86" s="108"/>
-      <c r="G86" s="108"/>
+      <c r="E86" s="109"/>
+      <c r="F86" s="109"/>
+      <c r="G86" s="109"/>
       <c r="H86" s="33"/>
       <c r="I86" s="8"/>
       <c r="J86" s="8"/>
@@ -15057,10 +15952,14 @@
         <v>23</v>
       </c>
       <c r="E87" s="81">
-        <v>0</v>
-      </c>
-      <c r="F87" s="82"/>
-      <c r="G87" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F87" s="82">
+        <v>44481</v>
+      </c>
+      <c r="G87" s="82">
+        <v>44484</v>
+      </c>
       <c r="H87" s="33"/>
       <c r="I87" s="8"/>
       <c r="J87" s="8"/>
@@ -15155,10 +16054,14 @@
         <v>137</v>
       </c>
       <c r="E88" s="81">
-        <v>0</v>
-      </c>
-      <c r="F88" s="82"/>
-      <c r="G88" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F88" s="82">
+        <v>44481</v>
+      </c>
+      <c r="G88" s="82">
+        <v>44484</v>
+      </c>
       <c r="H88" s="33"/>
       <c r="I88" s="8"/>
       <c r="J88" s="8"/>
@@ -15253,10 +16156,14 @@
         <v>18</v>
       </c>
       <c r="E89" s="81">
-        <v>0</v>
-      </c>
-      <c r="F89" s="82"/>
-      <c r="G89" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F89" s="82">
+        <v>44481</v>
+      </c>
+      <c r="G89" s="82">
+        <v>44484</v>
+      </c>
       <c r="H89" s="33"/>
       <c r="I89" s="8"/>
       <c r="J89" s="8"/>
@@ -15351,10 +16258,14 @@
         <v>17</v>
       </c>
       <c r="E90" s="81">
-        <v>0</v>
-      </c>
-      <c r="F90" s="82"/>
-      <c r="G90" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F90" s="82">
+        <v>44481</v>
+      </c>
+      <c r="G90" s="82">
+        <v>44484</v>
+      </c>
       <c r="H90" s="33"/>
       <c r="I90" s="8"/>
       <c r="J90" s="8"/>
@@ -15449,10 +16360,14 @@
         <v>64</v>
       </c>
       <c r="E91" s="81">
-        <v>0</v>
-      </c>
-      <c r="F91" s="82"/>
-      <c r="G91" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F91" s="82">
+        <v>44481</v>
+      </c>
+      <c r="G91" s="82">
+        <v>44484</v>
+      </c>
       <c r="H91" s="33"/>
       <c r="I91" s="8"/>
       <c r="J91" s="8"/>
@@ -15547,10 +16462,14 @@
         <v>24</v>
       </c>
       <c r="E92" s="81">
-        <v>0</v>
-      </c>
-      <c r="F92" s="82"/>
-      <c r="G92" s="82"/>
+        <v>1</v>
+      </c>
+      <c r="F92" s="82">
+        <v>44483</v>
+      </c>
+      <c r="G92" s="82">
+        <v>44484</v>
+      </c>
       <c r="H92" s="35"/>
       <c r="I92" s="36"/>
       <c r="J92" s="36"/>
@@ -15639,13 +16558,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="AD2:AJ2"/>
-    <mergeCell ref="D82:G82"/>
-    <mergeCell ref="D86:G86"/>
-    <mergeCell ref="D78:G78"/>
-    <mergeCell ref="D62:G62"/>
-    <mergeCell ref="D46:G46"/>
-    <mergeCell ref="D64:G64"/>
     <mergeCell ref="BT2:BZ2"/>
     <mergeCell ref="CA2:CG2"/>
     <mergeCell ref="CH2:CN2"/>
@@ -15662,6 +16574,13 @@
     <mergeCell ref="I2:O2"/>
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="W2:AC2"/>
+    <mergeCell ref="AD2:AJ2"/>
+    <mergeCell ref="D82:G82"/>
+    <mergeCell ref="D86:G86"/>
+    <mergeCell ref="D78:G78"/>
+    <mergeCell ref="D62:G62"/>
+    <mergeCell ref="D46:G46"/>
+    <mergeCell ref="D64:G64"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E10 E13:E16 E18:E24">
     <cfRule type="dataBar" priority="20">
@@ -15677,7 +16596,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E66:E77 E89:E92 E87:E88 E84:E85 E79:E81 E54:E61 E63 E50:E52 E35:E45 E47 E29:E33 E27">
+  <conditionalFormatting sqref="E29:E33 E27 E35:E45 E47 E50:E52 E54:E61 E63 E66:E77 E79:E81 E84:E85 E87:E92">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -15720,7 +16639,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E66:E77 E89:E92 E87:E88 E84:E85 E79:E81 E54:E61 E63 E50:E52 E35:E45 E47 E29:E33 E27</xm:sqref>
+          <xm:sqref>E29:E33 E27 E35:E45 E47 E50:E52 E54:E61 E63 E66:E77 E79:E81 E84:E85 E87:E92</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -15733,7 +16652,7 @@
   <dimension ref="A2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16011,16 +16930,16 @@
         <v>71</v>
       </c>
       <c r="F28" s="41">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="G28" s="41">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="H28" s="41">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="I28" s="41">
-        <v>0</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
@@ -16074,19 +16993,19 @@
       </c>
       <c r="F30" s="41" cm="1">
         <f t="array" ref="F30">SUM(D27:I27,-D28:F28)</f>
-        <v>223</v>
+        <v>140</v>
       </c>
       <c r="G30" s="41" cm="1">
         <f t="array" ref="G30">SUM(D27:I27,-D28:G28)</f>
-        <v>223</v>
+        <v>72</v>
       </c>
       <c r="H30" s="41" cm="1">
         <f t="array" ref="H30">SUM(D27:I27,-D28:H28)</f>
-        <v>223</v>
+        <v>7</v>
       </c>
       <c r="I30" s="41" cm="1">
         <f t="array" ref="I30">SUM(D27:I27,-D28:I28)</f>
-        <v>223</v>
+        <v>-48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expanded charts and added numbers
</commit_message>
<xml_diff>
--- a/documentation/Charts/Charts-WIP.xlsx
+++ b/documentation/Charts/Charts-WIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rex\Desktop\Project template code\Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115282E2-4E5B-4E8E-B7FB-6AA490CC7272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CDC2B3-8C95-42BB-8882-8C2C3C423B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{5FED8FEB-A2F0-45E6-B7D6-62982F9FC7E5}"/>
   </bookViews>
@@ -4426,8 +4426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3693011-238F-42BC-B2CC-2AF5AE5811AA}">
   <dimension ref="B4:M87"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6991,7 +6991,7 @@
   <dimension ref="A1:CN92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16652,7 +16652,7 @@
   <dimension ref="A2:J30"/>
   <sheetViews>
     <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F28" sqref="F28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>